<commit_message>
ignore compartments that aren't cellular in define_trajectory_classes
</commit_message>
<xml_diff>
--- a/tests/fixtures/dynamic_tests/one_exchange_rxn_compt_growth.xlsx
+++ b/tests/fixtures/dynamic_tests/one_exchange_rxn_compt_growth.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25620" yWindow="9180" windowWidth="25600" windowHeight="12420" tabRatio="500" firstSheet="6" activeTab="10"/>
-    <workbookView xWindow="0" yWindow="9640" windowWidth="31140" windowHeight="11840" tabRatio="500" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="-22820" yWindow="9960" windowWidth="22800" windowHeight="11640" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="540" yWindow="10140" windowWidth="37100" windowHeight="11200" tabRatio="500" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="247">
   <si>
     <t>!!!ObjTables ObjTablesVersion='0.0.8'</t>
   </si>
@@ -811,30 +811,6 @@
     <t>Exchange_reaction</t>
   </si>
   <si>
-    <t>!Compartment e mass</t>
-  </si>
-  <si>
-    <t>!Compartment e volume</t>
-  </si>
-  <si>
-    <t>!Compartment e accounted mass</t>
-  </si>
-  <si>
-    <t>!Compartment e accounted volume</t>
-  </si>
-  <si>
-    <t>Computation for Compartment e mass</t>
-  </si>
-  <si>
-    <t>Computation for Compartment e volume</t>
-  </si>
-  <si>
-    <t>Computation for Compartment e accounted mass</t>
-  </si>
-  <si>
-    <t>Computation for Compartment e accounted volume</t>
-  </si>
-  <si>
     <t>Computation for Pop A[e]</t>
   </si>
   <si>
@@ -848,6 +824,9 @@
   </si>
   <si>
     <t>volume(c) computed in expected_exponential_pops.py</t>
+  </si>
+  <si>
+    <t>Other expected values computed from volume or model parameters</t>
   </si>
 </sst>
 </file>
@@ -1931,7 +1910,7 @@
         <v>219</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>220</v>
@@ -1955,7 +1934,7 @@
         <v>20000</v>
       </c>
       <c r="F3" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1976,7 +1955,7 @@
         <v>19700</v>
       </c>
       <c r="F4" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2184,22 +2163,22 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="J3" sqref="J3:M15"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
-      <selection activeCell="Q15" sqref="Q3:Q15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>213</v>
       </c>
@@ -2215,7 +2194,7 @@
       <c r="K1" s="48"/>
       <c r="L1" s="48"/>
     </row>
-    <row r="2" spans="1:26" s="50" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="50" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
         <v>200</v>
       </c>
@@ -2268,34 +2247,10 @@
         <v>228</v>
       </c>
       <c r="R2" s="49" t="s">
-        <v>241</v>
-      </c>
-      <c r="S2" s="49" t="s">
-        <v>242</v>
-      </c>
-      <c r="T2" s="49" t="s">
-        <v>243</v>
-      </c>
-      <c r="U2" s="49" t="s">
-        <v>244</v>
-      </c>
-      <c r="V2" s="49" t="s">
-        <v>245</v>
-      </c>
-      <c r="W2" s="49" t="s">
-        <v>246</v>
-      </c>
-      <c r="X2" s="49" t="s">
-        <v>247</v>
-      </c>
-      <c r="Y2" s="49" t="s">
-        <v>248</v>
-      </c>
-      <c r="Z2" s="49" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2326,11 +2281,11 @@
         <f>P3 / density_c</f>
         <v>1.5095809458428766E-18</v>
       </c>
-      <c r="Z3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="R3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
@@ -2361,8 +2316,11 @@
         <f>P4 / density_c</f>
         <v>1.9624552295957395E-18</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="R4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20</v>
       </c>
@@ -2394,7 +2352,7 @@
         <v>2.4153295133486024E-18</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>30</v>
       </c>
@@ -2426,7 +2384,7 @@
         <v>3.1701199862700405E-18</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>40</v>
       </c>
@@ -2458,7 +2416,7 @@
         <v>4.0758685537757666E-18</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>50</v>
       </c>
@@ -2490,7 +2448,7 @@
         <v>5.2835333104500676E-18</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>60</v>
       </c>
@@ -2522,7 +2480,7 @@
         <v>6.7931142562929438E-18</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>70</v>
       </c>
@@ -2554,7 +2512,7 @@
         <v>8.604611391304396E-18</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>80</v>
       </c>
@@ -2586,7 +2544,7 @@
         <v>1.1170898999237286E-17</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>90</v>
       </c>
@@ -2618,7 +2576,7 @@
         <v>1.4341018985507327E-17</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>100</v>
       </c>
@@ -2650,7 +2608,7 @@
         <v>1.8416887539283093E-17</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>110</v>
       </c>
@@ -2682,7 +2640,7 @@
         <v>2.3549462755148872E-17</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>120</v>
       </c>
@@ -5053,7 +5011,7 @@
         <v>230</v>
       </c>
       <c r="D4" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E4" s="16">
         <v>0</v>
@@ -5372,7 +5330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
     <sheetView workbookViewId="1"/>

</xml_diff>

<commit_message>
improve comparison of floats in check_simul_results() by using only relative tolerance and math.isclose(); improve expected_exponential_pops.py with more accurate value for ACCOUNTED_FRACTION_C; fix expected trajectories in two models
</commit_message>
<xml_diff>
--- a/tests/fixtures/dynamic_tests/one_exchange_rxn_compt_growth.xlsx
+++ b/tests/fixtures/dynamic_tests/one_exchange_rxn_compt_growth.xlsx
@@ -1214,6 +1214,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1236,11 +1241,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1896,7 +1896,7 @@
       <c r="K1" s="43"/>
       <c r="L1" s="43"/>
     </row>
-    <row r="2" spans="1:12" s="70" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="61" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>200</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>1000</v>
       </c>
       <c r="E3">
-        <f>initial_pop_A_e - (D3 - initial_pop_A_c)</f>
+        <f t="shared" ref="E3:E15" si="0">initial_pop_A_e - (D3 - initial_pop_A_c)</f>
         <v>20000</v>
       </c>
       <c r="F3" t="s">
@@ -1951,7 +1951,7 @@
         <v>1300</v>
       </c>
       <c r="E4">
-        <f>initial_pop_A_e - (D4 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>19700</v>
       </c>
       <c r="F4" t="s">
@@ -1972,7 +1972,7 @@
         <v>1600</v>
       </c>
       <c r="E5">
-        <f>initial_pop_A_e - (D5 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>19400</v>
       </c>
     </row>
@@ -1990,7 +1990,7 @@
         <v>2100</v>
       </c>
       <c r="E6">
-        <f>initial_pop_A_e - (D6 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>18900</v>
       </c>
     </row>
@@ -2008,7 +2008,7 @@
         <v>2700</v>
       </c>
       <c r="E7">
-        <f>initial_pop_A_e - (D7 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>18300</v>
       </c>
     </row>
@@ -2026,7 +2026,7 @@
         <v>3500</v>
       </c>
       <c r="E8">
-        <f>initial_pop_A_e - (D8 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>17500</v>
       </c>
     </row>
@@ -2044,7 +2044,7 @@
         <v>4500</v>
       </c>
       <c r="E9">
-        <f>initial_pop_A_e - (D9 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>16500</v>
       </c>
     </row>
@@ -2062,7 +2062,7 @@
         <v>5700</v>
       </c>
       <c r="E10">
-        <f>initial_pop_A_e - (D10 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>15300</v>
       </c>
     </row>
@@ -2080,7 +2080,7 @@
         <v>7400</v>
       </c>
       <c r="E11">
-        <f>initial_pop_A_e - (D11 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>13600</v>
       </c>
     </row>
@@ -2098,7 +2098,7 @@
         <v>9500</v>
       </c>
       <c r="E12">
-        <f>initial_pop_A_e - (D12 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>11500</v>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
         <v>12200</v>
       </c>
       <c r="E13">
-        <f>initial_pop_A_e - (D13 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>8800</v>
       </c>
     </row>
@@ -2134,7 +2134,7 @@
         <v>15600</v>
       </c>
       <c r="E14">
-        <f>initial_pop_A_e - (D14 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>5400</v>
       </c>
     </row>
@@ -2152,7 +2152,7 @@
         <v>20100</v>
       </c>
       <c r="E15">
-        <f>initial_pop_A_e - (D15 - initial_pop_A_c)</f>
+        <f t="shared" si="0"/>
         <v>900</v>
       </c>
     </row>
@@ -2163,13 +2163,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="J3" sqref="J3:M15"/>
     </sheetView>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2178,7 +2178,7 @@
     <col min="18" max="18" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>213</v>
       </c>
@@ -2194,7 +2194,7 @@
       <c r="K1" s="48"/>
       <c r="L1" s="48"/>
     </row>
-    <row r="2" spans="1:18" s="50" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" s="50" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
         <v>200</v>
       </c>
@@ -2250,15 +2250,15 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
-      <c r="J3" s="69">
-        <v>1.0996947280000001E-14</v>
-      </c>
-      <c r="K3" s="69">
-        <v>9.9972248000000003E-18</v>
+      <c r="J3">
+        <v>1.1E-14</v>
+      </c>
+      <c r="K3">
+        <v>1.0000000000000001E-17</v>
       </c>
       <c r="L3">
         <v>1.6605390404271642E-15</v>
@@ -2266,34 +2266,38 @@
       <c r="M3">
         <v>1.5095809458428766E-18</v>
       </c>
-      <c r="N3" s="69">
-        <f>density_c * O3</f>
-        <v>1.0996947280000001E-14</v>
-      </c>
-      <c r="O3" s="69">
-        <v>9.9972248000000003E-18</v>
+      <c r="N3" s="60">
+        <f t="shared" ref="N3:N15" si="0">density_c * O3</f>
+        <v>1.1E-14</v>
+      </c>
+      <c r="O3" s="60">
+        <v>1.0000000000000001E-17</v>
       </c>
       <c r="P3">
         <f xml:space="preserve"> '!!Species trajectories'!D3 * Molecular_weight_A / avogadros_constant</f>
         <v>1.6605390404271642E-15</v>
       </c>
       <c r="Q3">
-        <f>P3 / density_c</f>
+        <f t="shared" ref="Q3:Q15" si="1">P3 / density_c</f>
         <v>1.5095809458428766E-18</v>
       </c>
       <c r="R3" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W3" s="60"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="60"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
-      <c r="J4" s="69">
-        <v>1.4296031200000001E-14</v>
-      </c>
-      <c r="K4" s="69">
-        <v>1.2996392E-17</v>
+      <c r="J4">
+        <v>1.43E-14</v>
+      </c>
+      <c r="K4">
+        <v>1.3E-17</v>
       </c>
       <c r="L4">
         <v>2.1587007525553134E-15</v>
@@ -2301,34 +2305,38 @@
       <c r="M4">
         <v>1.9624552295957395E-18</v>
       </c>
-      <c r="N4" s="69">
-        <f>density_c * O4</f>
-        <v>1.4296031200000001E-14</v>
-      </c>
-      <c r="O4" s="69">
-        <v>1.2996392E-17</v>
+      <c r="N4" s="60">
+        <f t="shared" si="0"/>
+        <v>1.43E-14</v>
+      </c>
+      <c r="O4" s="60">
+        <v>1.3E-17</v>
       </c>
       <c r="P4">
         <f xml:space="preserve"> '!!Species trajectories'!D4 * Molecular_weight_A / avogadros_constant</f>
         <v>2.1587007525553134E-15</v>
       </c>
       <c r="Q4">
-        <f>P4 / density_c</f>
+        <f t="shared" si="1"/>
         <v>1.9624552295957395E-18</v>
       </c>
       <c r="R4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W4" s="60"/>
+      <c r="X4" s="60"/>
+      <c r="Y4" s="60"/>
+      <c r="Z4" s="60"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20</v>
       </c>
-      <c r="J5" s="69">
-        <v>1.7595115999999998E-14</v>
-      </c>
-      <c r="K5" s="69">
-        <v>1.5995559999999999E-17</v>
+      <c r="J5">
+        <v>1.7600000000000002E-14</v>
+      </c>
+      <c r="K5">
+        <v>1.6000000000000001E-17</v>
       </c>
       <c r="L5">
         <v>2.6568624646834628E-15</v>
@@ -2336,31 +2344,35 @@
       <c r="M5">
         <v>2.4153295133486024E-18</v>
       </c>
-      <c r="N5" s="69">
-        <f>density_c * O5</f>
-        <v>1.7595115999999998E-14</v>
-      </c>
-      <c r="O5" s="69">
-        <v>1.5995559999999999E-17</v>
+      <c r="N5" s="60">
+        <f t="shared" si="0"/>
+        <v>1.7600000000000002E-14</v>
+      </c>
+      <c r="O5" s="60">
+        <v>1.6000000000000001E-17</v>
       </c>
       <c r="P5">
         <f xml:space="preserve"> '!!Species trajectories'!D5 * Molecular_weight_A / avogadros_constant</f>
         <v>2.6568624646834628E-15</v>
       </c>
       <c r="Q5">
-        <f>P5 / density_c</f>
+        <f t="shared" si="1"/>
         <v>2.4153295133486024E-18</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W5" s="60"/>
+      <c r="X5" s="60"/>
+      <c r="Y5" s="60"/>
+      <c r="Z5" s="60"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>30</v>
       </c>
-      <c r="J6" s="69">
-        <v>2.30935892E-14</v>
-      </c>
-      <c r="K6" s="69">
-        <v>2.0994172E-17</v>
+      <c r="J6">
+        <v>2.3100000000000001E-14</v>
+      </c>
+      <c r="K6">
+        <v>2.0999999999999999E-17</v>
       </c>
       <c r="L6">
         <v>3.4871319848970445E-15</v>
@@ -2368,31 +2380,35 @@
       <c r="M6">
         <v>3.1701199862700405E-18</v>
       </c>
-      <c r="N6" s="69">
-        <f>density_c * O6</f>
-        <v>2.30935892E-14</v>
-      </c>
-      <c r="O6" s="69">
-        <v>2.0994172E-17</v>
+      <c r="N6" s="60">
+        <f t="shared" si="0"/>
+        <v>2.3100000000000001E-14</v>
+      </c>
+      <c r="O6" s="60">
+        <v>2.0999999999999999E-17</v>
       </c>
       <c r="P6">
         <f xml:space="preserve"> '!!Species trajectories'!D6 * Molecular_weight_A / avogadros_constant</f>
         <v>3.4871319848970445E-15</v>
       </c>
       <c r="Q6">
-        <f>P6 / density_c</f>
+        <f t="shared" si="1"/>
         <v>3.1701199862700405E-18</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W6" s="60"/>
+      <c r="X6" s="60"/>
+      <c r="Y6" s="60"/>
+      <c r="Z6" s="60"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>40</v>
       </c>
-      <c r="J7" s="69">
-        <v>2.96917577E-14</v>
-      </c>
-      <c r="K7" s="69">
-        <v>2.6992507E-17</v>
+      <c r="J7">
+        <v>2.9700000000000002E-14</v>
+      </c>
+      <c r="K7">
+        <v>2.7000000000000001E-17</v>
       </c>
       <c r="L7">
         <v>4.4834554091533429E-15</v>
@@ -2400,31 +2416,35 @@
       <c r="M7">
         <v>4.0758685537757666E-18</v>
       </c>
-      <c r="N7" s="69">
-        <f>density_c * O7</f>
-        <v>2.96917577E-14</v>
-      </c>
-      <c r="O7" s="69">
-        <v>2.6992507E-17</v>
+      <c r="N7" s="60">
+        <f t="shared" si="0"/>
+        <v>2.9700000000000002E-14</v>
+      </c>
+      <c r="O7" s="60">
+        <v>2.7000000000000001E-17</v>
       </c>
       <c r="P7">
         <f xml:space="preserve"> '!!Species trajectories'!D7 * Molecular_weight_A / avogadros_constant</f>
         <v>4.4834554091533429E-15</v>
       </c>
       <c r="Q7">
-        <f>P7 / density_c</f>
+        <f t="shared" si="1"/>
         <v>4.0758685537757666E-18</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W7" s="60"/>
+      <c r="X7" s="60"/>
+      <c r="Y7" s="60"/>
+      <c r="Z7" s="60"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>50</v>
       </c>
-      <c r="J8" s="69">
-        <v>3.8489315700000002E-14</v>
-      </c>
-      <c r="K8" s="69">
-        <v>3.4990287000000003E-17</v>
+      <c r="J8">
+        <v>3.85E-14</v>
+      </c>
+      <c r="K8">
+        <v>3.5000000000000002E-17</v>
       </c>
       <c r="L8">
         <v>5.8118866414950741E-15</v>
@@ -2432,31 +2452,35 @@
       <c r="M8">
         <v>5.2835333104500676E-18</v>
       </c>
-      <c r="N8" s="69">
-        <f>density_c * O8</f>
-        <v>3.8489315700000002E-14</v>
-      </c>
-      <c r="O8" s="69">
-        <v>3.4990287000000003E-17</v>
+      <c r="N8" s="60">
+        <f t="shared" si="0"/>
+        <v>3.85E-14</v>
+      </c>
+      <c r="O8" s="60">
+        <v>3.5000000000000002E-17</v>
       </c>
       <c r="P8">
         <f xml:space="preserve"> '!!Species trajectories'!D8 * Molecular_weight_A / avogadros_constant</f>
         <v>5.8118866414950741E-15</v>
       </c>
       <c r="Q8">
-        <f>P8 / density_c</f>
+        <f t="shared" si="1"/>
         <v>5.2835333104500676E-18</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W8" s="60"/>
+      <c r="X8" s="60"/>
+      <c r="Y8" s="60"/>
+      <c r="Z8" s="60"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>60</v>
       </c>
-      <c r="J9" s="69">
-        <v>4.9486263199999997E-14</v>
-      </c>
-      <c r="K9" s="69">
-        <v>4.4987511999999999E-17</v>
+      <c r="J9">
+        <v>4.9499999999999997E-14</v>
+      </c>
+      <c r="K9">
+        <v>4.4999999999999998E-17</v>
       </c>
       <c r="L9">
         <v>7.4724256819222385E-15</v>
@@ -2464,31 +2488,35 @@
       <c r="M9">
         <v>6.7931142562929438E-18</v>
       </c>
-      <c r="N9" s="69">
-        <f>density_c * O9</f>
-        <v>4.9486263199999997E-14</v>
-      </c>
-      <c r="O9" s="69">
-        <v>4.4987511999999999E-17</v>
+      <c r="N9" s="60">
+        <f t="shared" si="0"/>
+        <v>4.9499999999999997E-14</v>
+      </c>
+      <c r="O9" s="60">
+        <v>4.4999999999999998E-17</v>
       </c>
       <c r="P9">
         <f xml:space="preserve"> '!!Species trajectories'!D9 * Molecular_weight_A / avogadros_constant</f>
         <v>7.4724256819222385E-15</v>
       </c>
       <c r="Q9">
-        <f>P9 / density_c</f>
+        <f t="shared" si="1"/>
         <v>6.7931142562929438E-18</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W9" s="60"/>
+      <c r="X9" s="60"/>
+      <c r="Y9" s="60"/>
+      <c r="Z9" s="60"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>70</v>
       </c>
-      <c r="J10" s="69">
-        <v>6.2682599099999994E-14</v>
-      </c>
-      <c r="K10" s="69">
-        <v>5.6984180999999998E-17</v>
+      <c r="J10">
+        <v>6.27E-14</v>
+      </c>
+      <c r="K10">
+        <v>5.7000000000000002E-17</v>
       </c>
       <c r="L10">
         <v>9.465072530434836E-15</v>
@@ -2496,31 +2524,35 @@
       <c r="M10">
         <v>8.604611391304396E-18</v>
       </c>
-      <c r="N10" s="69">
-        <f>density_c * O10</f>
-        <v>6.2682599099999994E-14</v>
-      </c>
-      <c r="O10" s="69">
-        <v>5.6984180999999998E-17</v>
+      <c r="N10" s="60">
+        <f t="shared" si="0"/>
+        <v>6.27E-14</v>
+      </c>
+      <c r="O10" s="60">
+        <v>5.7000000000000002E-17</v>
       </c>
       <c r="P10">
         <f xml:space="preserve"> '!!Species trajectories'!D10 * Molecular_weight_A / avogadros_constant</f>
         <v>9.465072530434836E-15</v>
       </c>
       <c r="Q10">
-        <f>P10 / density_c</f>
+        <f t="shared" si="1"/>
         <v>8.604611391304396E-18</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W10" s="60"/>
+      <c r="X10" s="60"/>
+      <c r="Y10" s="60"/>
+      <c r="Z10" s="60"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>80</v>
       </c>
-      <c r="J11" s="69">
-        <v>8.1377410400000002E-14</v>
-      </c>
-      <c r="K11" s="69">
-        <v>7.3979463999999999E-17</v>
+      <c r="J11">
+        <v>8.1399999999999999E-14</v>
+      </c>
+      <c r="K11">
+        <v>7.3999999999999995E-17</v>
       </c>
       <c r="L11">
         <v>1.2287988899161015E-14</v>
@@ -2528,31 +2560,35 @@
       <c r="M11">
         <v>1.1170898999237286E-17</v>
       </c>
-      <c r="N11" s="69">
-        <f>density_c * O11</f>
-        <v>8.1377410400000002E-14</v>
-      </c>
-      <c r="O11" s="69">
-        <v>7.3979463999999999E-17</v>
+      <c r="N11" s="60">
+        <f t="shared" si="0"/>
+        <v>8.1399999999999999E-14</v>
+      </c>
+      <c r="O11" s="60">
+        <v>7.3999999999999995E-17</v>
       </c>
       <c r="P11">
         <f xml:space="preserve"> '!!Species trajectories'!D11 * Molecular_weight_A / avogadros_constant</f>
         <v>1.2287988899161015E-14</v>
       </c>
       <c r="Q11">
-        <f>P11 / density_c</f>
+        <f t="shared" si="1"/>
         <v>1.1170898999237286E-17</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W11" s="60"/>
+      <c r="X11" s="60"/>
+      <c r="Y11" s="60"/>
+      <c r="Z11" s="60"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>90</v>
       </c>
-      <c r="J12" s="69">
-        <v>1.044709996E-13</v>
-      </c>
-      <c r="K12" s="69">
-        <v>9.4973635999999999E-17</v>
+      <c r="J12">
+        <v>1.0450000000000001E-13</v>
+      </c>
+      <c r="K12">
+        <v>9.5000000000000003E-17</v>
       </c>
       <c r="L12">
         <v>1.577512088405806E-14</v>
@@ -2560,31 +2596,35 @@
       <c r="M12">
         <v>1.4341018985507327E-17</v>
       </c>
-      <c r="N12" s="69">
-        <f>density_c * O12</f>
-        <v>1.044709996E-13</v>
-      </c>
-      <c r="O12" s="69">
-        <v>9.4973635999999999E-17</v>
+      <c r="N12" s="60">
+        <f t="shared" si="0"/>
+        <v>1.0450000000000001E-13</v>
+      </c>
+      <c r="O12" s="60">
+        <v>9.5000000000000003E-17</v>
       </c>
       <c r="P12">
         <f xml:space="preserve"> '!!Species trajectories'!D12 * Molecular_weight_A / avogadros_constant</f>
         <v>1.577512088405806E-14</v>
       </c>
       <c r="Q12">
-        <f>P12 / density_c</f>
+        <f t="shared" si="1"/>
         <v>1.4341018985507327E-17</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W12" s="60"/>
+      <c r="X12" s="60"/>
+      <c r="Y12" s="60"/>
+      <c r="Z12" s="60"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>100</v>
       </c>
-      <c r="J13" s="69">
-        <v>1.34162754E-13</v>
-      </c>
-      <c r="K13" s="69">
-        <v>1.2196613999999999E-16</v>
+      <c r="J13">
+        <v>1.3420000000000002E-13</v>
+      </c>
+      <c r="K13">
+        <v>1.2200000000000001E-16</v>
       </c>
       <c r="L13">
         <v>2.0258576293211402E-14</v>
@@ -2592,31 +2632,35 @@
       <c r="M13">
         <v>1.8416887539283093E-17</v>
       </c>
-      <c r="N13" s="69">
-        <f>density_c * O13</f>
-        <v>1.34162754E-13</v>
-      </c>
-      <c r="O13" s="69">
-        <v>1.2196613999999999E-16</v>
+      <c r="N13" s="60">
+        <f t="shared" si="0"/>
+        <v>1.3420000000000002E-13</v>
+      </c>
+      <c r="O13" s="60">
+        <v>1.2200000000000001E-16</v>
       </c>
       <c r="P13">
         <f xml:space="preserve"> '!!Species trajectories'!D13 * Molecular_weight_A / avogadros_constant</f>
         <v>2.0258576293211402E-14</v>
       </c>
       <c r="Q13">
-        <f>P13 / density_c</f>
+        <f t="shared" si="1"/>
         <v>1.8416887539283093E-17</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W13" s="60"/>
+      <c r="X13" s="60"/>
+      <c r="Y13" s="60"/>
+      <c r="Z13" s="60"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>110</v>
       </c>
-      <c r="J14" s="69">
-        <v>1.7155238100000001E-13</v>
-      </c>
-      <c r="K14" s="69">
-        <v>1.5595671E-16</v>
+      <c r="J14">
+        <v>1.716E-13</v>
+      </c>
+      <c r="K14">
+        <v>1.56E-16</v>
       </c>
       <c r="L14">
         <v>2.5904409030663759E-14</v>
@@ -2624,31 +2668,35 @@
       <c r="M14">
         <v>2.3549462755148872E-17</v>
       </c>
-      <c r="N14" s="69">
-        <f>density_c * O14</f>
-        <v>1.7155238100000001E-13</v>
-      </c>
-      <c r="O14" s="69">
-        <v>1.5595671E-16</v>
+      <c r="N14" s="60">
+        <f t="shared" si="0"/>
+        <v>1.716E-13</v>
+      </c>
+      <c r="O14" s="60">
+        <v>1.56E-16</v>
       </c>
       <c r="P14">
         <f xml:space="preserve"> '!!Species trajectories'!D14 * Molecular_weight_A / avogadros_constant</f>
         <v>2.5904409030663759E-14</v>
       </c>
       <c r="Q14">
-        <f>P14 / density_c</f>
+        <f t="shared" si="1"/>
         <v>2.3549462755148872E-17</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W14" s="60"/>
+      <c r="X14" s="60"/>
+      <c r="Y14" s="60"/>
+      <c r="Z14" s="60"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>120</v>
       </c>
-      <c r="J15" s="69">
-        <v>2.2103864199999999E-13</v>
-      </c>
-      <c r="K15" s="69">
-        <v>2.0094422E-16</v>
+      <c r="J15">
+        <v>2.2110000000000001E-13</v>
+      </c>
+      <c r="K15">
+        <v>2.0100000000000001E-16</v>
       </c>
       <c r="L15">
         <v>3.3376834712585996E-14</v>
@@ -2656,21 +2704,25 @@
       <c r="M15">
         <v>3.0342577011441815E-17</v>
       </c>
-      <c r="N15" s="69">
-        <f>density_c * O15</f>
-        <v>2.2103864199999999E-13</v>
-      </c>
-      <c r="O15" s="69">
-        <v>2.0094422E-16</v>
+      <c r="N15" s="60">
+        <f t="shared" si="0"/>
+        <v>2.2110000000000001E-13</v>
+      </c>
+      <c r="O15" s="60">
+        <v>2.0100000000000001E-16</v>
       </c>
       <c r="P15">
         <f xml:space="preserve"> '!!Species trajectories'!D15 * Molecular_weight_A / avogadros_constant</f>
         <v>3.3376834712585996E-14</v>
       </c>
       <c r="Q15">
-        <f>P15 / density_c</f>
+        <f t="shared" si="1"/>
         <v>3.0342577011441815E-17</v>
       </c>
+      <c r="W15" s="60"/>
+      <c r="X15" s="60"/>
+      <c r="Y15" s="60"/>
+      <c r="Z15" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2794,7 +2846,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="59" t="s">
         <v>108</v>
       </c>
       <c r="B1" s="58"/>
@@ -2853,21 +2905,21 @@
       <c r="I3" s="58"/>
     </row>
     <row r="4" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2919,11 +2971,11 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -5535,7 +5587,7 @@
       <c r="C4" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="69">
+      <c r="D4" s="60">
         <v>2.5E+16</v>
       </c>
       <c r="E4"/>
@@ -5704,26 +5756,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="66" t="s">
+      <c r="G2" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="H2" s="64"/>
-      <c r="I2" s="66" t="s">
+      <c r="H2" s="67"/>
+      <c r="I2" s="69" t="s">
         <v>148</v>
       </c>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="Q2" s="67" t="s">
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="Q2" s="70" t="s">
         <v>149</v>
       </c>
-      <c r="R2" s="64"/>
-      <c r="S2" s="67" t="s">
+      <c r="R2" s="67"/>
+      <c r="S2" s="70" t="s">
         <v>150</v>
       </c>
-      <c r="T2" s="64"/>
+      <c r="T2" s="67"/>
     </row>
     <row r="3" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5889,10 +5941,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="H2" s="64"/>
+      <c r="H2" s="67"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -6488,19 +6540,19 @@
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
       <c r="G2" s="32"/>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="61"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
       <c r="L2" s="32"/>
-      <c r="M2" s="62" t="s">
+      <c r="M2" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -8619,7 +8671,7 @@
       <c r="H4" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="69">
+      <c r="I4" s="60">
         <v>1.0000000000000001E-17</v>
       </c>
       <c r="J4" s="34"/>
@@ -8739,14 +8791,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -8803,7 +8855,7 @@
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
-      <c r="G4" s="69">
+      <c r="G4" s="60">
         <v>1000000</v>
       </c>
       <c r="H4" s="16">

</xml_diff>

<commit_message>
have DynamicSpecies use the right interface to LocalSpeciesPopulation; add unit tests of DynamicSpecies to tests/fixtures/test_dynamic_expressions.xlsx; resave changes in dynamic_tests/one_exchange_rxn_compt_growth.xlsx
</commit_message>
<xml_diff>
--- a/tests/fixtures/dynamic_tests/one_exchange_rxn_compt_growth.xlsx
+++ b/tests/fixtures/dynamic_tests/one_exchange_rxn_compt_growth.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-22820" yWindow="9960" windowWidth="22800" windowHeight="11640" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-21740" yWindow="10600" windowWidth="21720" windowHeight="11000" tabRatio="500" firstSheet="1" activeTab="1"/>
     <workbookView xWindow="540" yWindow="10140" windowWidth="37100" windowHeight="11200" tabRatio="500" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
@@ -2169,7 +2169,7 @@
       <selection activeCell="J3" sqref="J3:M15"/>
     </sheetView>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J3" sqref="J3:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2254,10 +2254,10 @@
       <c r="A3">
         <v>0</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="60">
         <v>1.1E-14</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="60">
         <v>1.0000000000000001E-17</v>
       </c>
       <c r="L3">
@@ -2293,10 +2293,10 @@
       <c r="A4">
         <v>10</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="60">
         <v>1.43E-14</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="60">
         <v>1.3E-17</v>
       </c>
       <c r="L4">
@@ -2332,10 +2332,10 @@
       <c r="A5">
         <v>20</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="60">
         <v>1.7600000000000002E-14</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="60">
         <v>1.6000000000000001E-17</v>
       </c>
       <c r="L5">
@@ -2368,10 +2368,10 @@
       <c r="A6">
         <v>30</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="60">
         <v>2.3100000000000001E-14</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="60">
         <v>2.0999999999999999E-17</v>
       </c>
       <c r="L6">
@@ -2404,10 +2404,10 @@
       <c r="A7">
         <v>40</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="60">
         <v>2.9700000000000002E-14</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="60">
         <v>2.7000000000000001E-17</v>
       </c>
       <c r="L7">
@@ -2440,10 +2440,10 @@
       <c r="A8">
         <v>50</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="60">
         <v>3.85E-14</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="60">
         <v>3.5000000000000002E-17</v>
       </c>
       <c r="L8">
@@ -2476,10 +2476,10 @@
       <c r="A9">
         <v>60</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="60">
         <v>4.9499999999999997E-14</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="60">
         <v>4.4999999999999998E-17</v>
       </c>
       <c r="L9">
@@ -2512,10 +2512,10 @@
       <c r="A10">
         <v>70</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="60">
         <v>6.27E-14</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="60">
         <v>5.7000000000000002E-17</v>
       </c>
       <c r="L10">
@@ -2548,10 +2548,10 @@
       <c r="A11">
         <v>80</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="60">
         <v>8.1399999999999999E-14</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="60">
         <v>7.3999999999999995E-17</v>
       </c>
       <c r="L11">
@@ -2584,10 +2584,10 @@
       <c r="A12">
         <v>90</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="60">
         <v>1.0450000000000001E-13</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="60">
         <v>9.5000000000000003E-17</v>
       </c>
       <c r="L12">
@@ -2620,10 +2620,10 @@
       <c r="A13">
         <v>100</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="60">
         <v>1.3420000000000002E-13</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="60">
         <v>1.2200000000000001E-16</v>
       </c>
       <c r="L13">
@@ -2656,10 +2656,10 @@
       <c r="A14">
         <v>110</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="60">
         <v>1.716E-13</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="60">
         <v>1.56E-16</v>
       </c>
       <c r="L14">
@@ -2692,10 +2692,10 @@
       <c r="A15">
         <v>120</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="60">
         <v>2.2110000000000001E-13</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="60">
         <v>2.0100000000000001E-16</v>
       </c>
       <c r="L15">
@@ -5383,7 +5383,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>

</xml_diff>

<commit_message>
dynamic test that passes
</commit_message>
<xml_diff>
--- a/tests/fixtures/dynamic_tests/one_exchange_rxn_compt_growth.xlsx
+++ b/tests/fixtures/dynamic_tests/one_exchange_rxn_compt_growth.xlsx
@@ -9,8 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="540" yWindow="4360" windowWidth="37100" windowHeight="16980" tabRatio="500" firstSheet="8" activeTab="10"/>
-    <workbookView xWindow="-21420" yWindow="11500" windowWidth="21140" windowHeight="9960" tabRatio="500" firstSheet="11" activeTab="18"/>
+    <workbookView xWindow="-11260" yWindow="22420" windowWidth="21140" windowHeight="9960" tabRatio="500" firstSheet="11" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -822,8 +821,8 @@
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="0.0E+00"/>
     <numFmt numFmtId="167" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="173" formatCode="0.00000000000E+00"/>
-    <numFmt numFmtId="174" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.00000000000E+00"/>
+    <numFmt numFmtId="169" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1167,6 +1166,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1190,9 +1192,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -1543,7 +1542,6 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1814,10 +1812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1886,7 +1881,7 @@
       </c>
       <c r="H3" s="57"/>
       <c r="I3" s="57"/>
-      <c r="J3" s="70"/>
+      <c r="J3" s="61"/>
       <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1911,7 +1906,7 @@
       </c>
       <c r="H4" s="57"/>
       <c r="I4" s="57"/>
-      <c r="J4" s="70"/>
+      <c r="J4" s="61"/>
       <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1933,7 +1928,7 @@
       </c>
       <c r="H5" s="57"/>
       <c r="I5" s="57"/>
-      <c r="J5" s="70"/>
+      <c r="J5" s="61"/>
       <c r="K5" s="57"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1955,7 +1950,7 @@
       </c>
       <c r="H6" s="57"/>
       <c r="I6" s="57"/>
-      <c r="J6" s="70"/>
+      <c r="J6" s="61"/>
       <c r="K6" s="57"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1977,7 +1972,7 @@
       </c>
       <c r="H7" s="57"/>
       <c r="I7" s="57"/>
-      <c r="J7" s="70"/>
+      <c r="J7" s="61"/>
       <c r="K7" s="57"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1999,7 +1994,7 @@
       </c>
       <c r="H8" s="57"/>
       <c r="I8" s="57"/>
-      <c r="J8" s="70"/>
+      <c r="J8" s="61"/>
       <c r="K8" s="57"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -2021,7 +2016,7 @@
       </c>
       <c r="H9" s="57"/>
       <c r="I9" s="57"/>
-      <c r="J9" s="70"/>
+      <c r="J9" s="61"/>
       <c r="K9" s="57"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -2043,7 +2038,7 @@
       </c>
       <c r="H10" s="57"/>
       <c r="I10" s="57"/>
-      <c r="J10" s="70"/>
+      <c r="J10" s="61"/>
       <c r="K10" s="57"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -2065,7 +2060,7 @@
       </c>
       <c r="H11" s="57"/>
       <c r="I11" s="57"/>
-      <c r="J11" s="70"/>
+      <c r="J11" s="61"/>
       <c r="K11" s="57"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -2087,7 +2082,7 @@
       </c>
       <c r="H12" s="57"/>
       <c r="I12" s="57"/>
-      <c r="J12" s="70"/>
+      <c r="J12" s="61"/>
       <c r="K12" s="57"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -2109,7 +2104,7 @@
       </c>
       <c r="H13" s="57"/>
       <c r="I13" s="57"/>
-      <c r="J13" s="70"/>
+      <c r="J13" s="61"/>
       <c r="K13" s="57"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -2131,7 +2126,7 @@
       </c>
       <c r="H14" s="57"/>
       <c r="I14" s="57"/>
-      <c r="J14" s="70"/>
+      <c r="J14" s="61"/>
       <c r="K14" s="57"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -2153,7 +2148,7 @@
       </c>
       <c r="H15" s="57"/>
       <c r="I15" s="57"/>
-      <c r="J15" s="70"/>
+      <c r="J15" s="61"/>
       <c r="K15" s="57"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -2173,7 +2168,7 @@
         <f t="shared" si="0"/>
         <v>19080</v>
       </c>
-      <c r="J16" s="70"/>
+      <c r="J16" s="61"/>
       <c r="K16" s="57"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -2193,7 +2188,7 @@
         <f t="shared" si="0"/>
         <v>18990</v>
       </c>
-      <c r="J17" s="70"/>
+      <c r="J17" s="61"/>
       <c r="K17" s="57"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -2213,7 +2208,7 @@
         <f t="shared" si="0"/>
         <v>18880</v>
       </c>
-      <c r="J18" s="70"/>
+      <c r="J18" s="61"/>
       <c r="K18" s="57"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -2233,7 +2228,7 @@
         <f t="shared" si="0"/>
         <v>18770</v>
       </c>
-      <c r="J19" s="70"/>
+      <c r="J19" s="61"/>
       <c r="K19" s="57"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -2253,7 +2248,7 @@
         <f t="shared" si="0"/>
         <v>18660</v>
       </c>
-      <c r="J20" s="70"/>
+      <c r="J20" s="61"/>
       <c r="K20" s="57"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -2273,7 +2268,7 @@
         <f t="shared" si="0"/>
         <v>18540</v>
       </c>
-      <c r="J21" s="70"/>
+      <c r="J21" s="61"/>
       <c r="K21" s="57"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -2293,7 +2288,7 @@
         <f t="shared" si="0"/>
         <v>18410</v>
       </c>
-      <c r="J22" s="70"/>
+      <c r="J22" s="61"/>
       <c r="K22" s="57"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -2313,7 +2308,7 @@
         <f t="shared" si="0"/>
         <v>18280</v>
       </c>
-      <c r="J23" s="70"/>
+      <c r="J23" s="61"/>
       <c r="K23" s="57"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -2333,7 +2328,7 @@
         <f t="shared" si="0"/>
         <v>18140</v>
       </c>
-      <c r="J24" s="70"/>
+      <c r="J24" s="61"/>
       <c r="K24" s="57"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -2353,7 +2348,7 @@
         <f t="shared" si="0"/>
         <v>18000</v>
       </c>
-      <c r="J25" s="70"/>
+      <c r="J25" s="61"/>
       <c r="K25" s="57"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -2373,7 +2368,7 @@
         <f t="shared" si="0"/>
         <v>17840</v>
       </c>
-      <c r="J26" s="70"/>
+      <c r="J26" s="61"/>
       <c r="K26" s="57"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -2393,7 +2388,7 @@
         <f t="shared" si="0"/>
         <v>17680</v>
       </c>
-      <c r="J27" s="70"/>
+      <c r="J27" s="61"/>
       <c r="K27" s="57"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -2413,7 +2408,7 @@
         <f t="shared" si="0"/>
         <v>17510</v>
       </c>
-      <c r="J28" s="70"/>
+      <c r="J28" s="61"/>
       <c r="K28" s="57"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -2433,7 +2428,7 @@
         <f t="shared" si="0"/>
         <v>17330</v>
       </c>
-      <c r="J29" s="70"/>
+      <c r="J29" s="61"/>
       <c r="K29" s="57"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -2453,7 +2448,7 @@
         <f t="shared" si="0"/>
         <v>17140</v>
       </c>
-      <c r="J30" s="70"/>
+      <c r="J30" s="61"/>
       <c r="K30" s="57"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -2473,7 +2468,7 @@
         <f t="shared" si="0"/>
         <v>16940</v>
       </c>
-      <c r="J31" s="70"/>
+      <c r="J31" s="61"/>
       <c r="K31" s="57"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -2493,7 +2488,7 @@
         <f t="shared" si="0"/>
         <v>16740</v>
       </c>
-      <c r="J32" s="70"/>
+      <c r="J32" s="61"/>
       <c r="K32" s="57"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -2513,7 +2508,7 @@
         <f t="shared" si="0"/>
         <v>16520</v>
       </c>
-      <c r="J33" s="70"/>
+      <c r="J33" s="61"/>
       <c r="K33" s="57"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -2533,7 +2528,7 @@
         <f t="shared" si="0"/>
         <v>16290</v>
       </c>
-      <c r="J34" s="70"/>
+      <c r="J34" s="61"/>
       <c r="K34" s="57"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -2553,7 +2548,7 @@
         <f t="shared" si="0"/>
         <v>16050</v>
       </c>
-      <c r="J35" s="70"/>
+      <c r="J35" s="61"/>
       <c r="K35" s="57"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -2573,7 +2568,7 @@
         <f t="shared" si="0"/>
         <v>15790</v>
       </c>
-      <c r="J36" s="70"/>
+      <c r="J36" s="61"/>
       <c r="K36" s="57"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -2593,7 +2588,7 @@
         <f t="shared" si="0"/>
         <v>15530</v>
       </c>
-      <c r="J37" s="70"/>
+      <c r="J37" s="61"/>
       <c r="K37" s="57"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -2613,7 +2608,7 @@
         <f t="shared" si="0"/>
         <v>15250</v>
       </c>
-      <c r="J38" s="70"/>
+      <c r="J38" s="61"/>
       <c r="K38" s="57"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -2633,7 +2628,7 @@
         <f t="shared" si="0"/>
         <v>14950</v>
       </c>
-      <c r="J39" s="70"/>
+      <c r="J39" s="61"/>
       <c r="K39" s="57"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -2653,7 +2648,7 @@
         <f t="shared" si="0"/>
         <v>14640</v>
       </c>
-      <c r="J40" s="70"/>
+      <c r="J40" s="61"/>
       <c r="K40" s="57"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2673,7 +2668,7 @@
         <f t="shared" si="0"/>
         <v>14310</v>
       </c>
-      <c r="J41" s="70"/>
+      <c r="J41" s="61"/>
       <c r="K41" s="57"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -2693,7 +2688,7 @@
         <f t="shared" si="0"/>
         <v>13970</v>
       </c>
-      <c r="J42" s="70"/>
+      <c r="J42" s="61"/>
       <c r="K42" s="57"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -2713,7 +2708,7 @@
         <f t="shared" si="0"/>
         <v>13610</v>
       </c>
-      <c r="J43" s="70"/>
+      <c r="J43" s="61"/>
       <c r="K43" s="57"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -2733,7 +2728,7 @@
         <f t="shared" si="0"/>
         <v>13230</v>
       </c>
-      <c r="J44" s="70"/>
+      <c r="J44" s="61"/>
       <c r="K44" s="57"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -2753,7 +2748,7 @@
         <f t="shared" si="0"/>
         <v>12830</v>
       </c>
-      <c r="J45" s="70"/>
+      <c r="J45" s="61"/>
       <c r="K45" s="57"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -2773,7 +2768,7 @@
         <f t="shared" si="0"/>
         <v>12420</v>
       </c>
-      <c r="J46" s="70"/>
+      <c r="J46" s="61"/>
       <c r="K46" s="57"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -2793,7 +2788,7 @@
         <f t="shared" si="0"/>
         <v>11980</v>
       </c>
-      <c r="J47" s="70"/>
+      <c r="J47" s="61"/>
       <c r="K47" s="57"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -2813,7 +2808,7 @@
         <f t="shared" si="0"/>
         <v>11510</v>
       </c>
-      <c r="J48" s="70"/>
+      <c r="J48" s="61"/>
       <c r="K48" s="57"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -2833,7 +2828,7 @@
         <f t="shared" si="0"/>
         <v>11030</v>
       </c>
-      <c r="J49" s="70"/>
+      <c r="J49" s="61"/>
       <c r="K49" s="57"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2853,7 +2848,7 @@
         <f t="shared" si="0"/>
         <v>10510</v>
       </c>
-      <c r="J50" s="70"/>
+      <c r="J50" s="61"/>
       <c r="K50" s="57"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -2873,7 +2868,7 @@
         <f t="shared" si="0"/>
         <v>9980</v>
       </c>
-      <c r="J51" s="70"/>
+      <c r="J51" s="61"/>
       <c r="K51" s="57"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -2893,7 +2888,7 @@
         <f t="shared" si="0"/>
         <v>9410</v>
       </c>
-      <c r="J52" s="70"/>
+      <c r="J52" s="61"/>
       <c r="K52" s="57"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -2913,7 +2908,7 @@
         <f t="shared" si="0"/>
         <v>8820</v>
       </c>
-      <c r="J53" s="70"/>
+      <c r="J53" s="61"/>
       <c r="K53" s="57"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2933,7 +2928,7 @@
         <f t="shared" si="0"/>
         <v>8190</v>
       </c>
-      <c r="J54" s="70"/>
+      <c r="J54" s="61"/>
       <c r="K54" s="57"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -2953,7 +2948,7 @@
         <f t="shared" si="0"/>
         <v>7540</v>
       </c>
-      <c r="J55" s="70"/>
+      <c r="J55" s="61"/>
       <c r="K55" s="57"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -2973,7 +2968,7 @@
         <f t="shared" si="0"/>
         <v>6850</v>
       </c>
-      <c r="J56" s="70"/>
+      <c r="J56" s="61"/>
       <c r="K56" s="57"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -2993,7 +2988,7 @@
         <f t="shared" si="0"/>
         <v>6120</v>
       </c>
-      <c r="J57" s="70"/>
+      <c r="J57" s="61"/>
       <c r="K57" s="57"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -3013,7 +3008,7 @@
         <f t="shared" si="0"/>
         <v>5360</v>
       </c>
-      <c r="J58" s="70"/>
+      <c r="J58" s="61"/>
       <c r="K58" s="57"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -3033,7 +3028,7 @@
         <f t="shared" si="0"/>
         <v>4560</v>
       </c>
-      <c r="J59" s="70"/>
+      <c r="J59" s="61"/>
       <c r="K59" s="57"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -3053,7 +3048,7 @@
         <f t="shared" si="0"/>
         <v>3710</v>
       </c>
-      <c r="J60" s="70"/>
+      <c r="J60" s="61"/>
       <c r="K60" s="57"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -3073,7 +3068,7 @@
         <f t="shared" si="0"/>
         <v>2830</v>
       </c>
-      <c r="J61" s="70"/>
+      <c r="J61" s="61"/>
       <c r="K61" s="57"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -3093,7 +3088,7 @@
         <f t="shared" si="0"/>
         <v>1890</v>
       </c>
-      <c r="J62" s="70"/>
+      <c r="J62" s="61"/>
       <c r="K62" s="57"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -3113,7 +3108,7 @@
         <f t="shared" si="0"/>
         <v>910</v>
       </c>
-      <c r="J63" s="70"/>
+      <c r="J63" s="61"/>
       <c r="K63" s="57"/>
     </row>
   </sheetData>
@@ -3125,12 +3120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="2080" topLeftCell="A3" activePane="bottomLeft"/>
-      <selection activeCell="V1" sqref="V1:V1048576"/>
-      <selection pane="bottomLeft" activeCell="R4" sqref="R4"/>
-    </sheetView>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3215,10 +3205,10 @@
       <c r="A3">
         <v>0</v>
       </c>
-      <c r="J3" s="68">
+      <c r="J3" s="59">
         <v>1.1E-14</v>
       </c>
-      <c r="K3" s="68">
+      <c r="K3" s="59">
         <v>1.0000000000000001E-17</v>
       </c>
       <c r="L3">
@@ -3227,11 +3217,11 @@
       <c r="M3">
         <v>1.5095809458428766E-18</v>
       </c>
-      <c r="N3" s="68">
+      <c r="N3" s="59">
         <f t="shared" ref="N3:N63" si="0">density_c * O3</f>
         <v>1.1E-14</v>
       </c>
-      <c r="O3" s="70">
+      <c r="O3" s="61">
         <v>1.0000000000000001E-17</v>
       </c>
       <c r="P3">
@@ -3247,17 +3237,17 @@
       </c>
       <c r="T3" s="57"/>
       <c r="U3" s="57"/>
-      <c r="V3" s="70"/>
+      <c r="V3" s="61"/>
       <c r="W3" s="57"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="J4" s="68">
+      <c r="J4" s="59">
         <v>1.155E-14</v>
       </c>
-      <c r="K4" s="68">
+      <c r="K4" s="59">
         <v>1.05E-17</v>
       </c>
       <c r="L4">
@@ -3266,11 +3256,11 @@
       <c r="M4">
         <v>1.5850599931350202E-18</v>
       </c>
-      <c r="N4" s="68">
+      <c r="N4" s="59">
         <f t="shared" si="0"/>
         <v>1.155E-14</v>
       </c>
-      <c r="O4" s="70">
+      <c r="O4" s="61">
         <v>1.05E-17</v>
       </c>
       <c r="P4">
@@ -3286,17 +3276,17 @@
       </c>
       <c r="T4" s="57"/>
       <c r="U4" s="57"/>
-      <c r="V4" s="70"/>
+      <c r="V4" s="61"/>
       <c r="W4" s="57"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="J5" s="68">
+      <c r="J5" s="59">
         <v>1.2209999999999999E-14</v>
       </c>
-      <c r="K5" s="68">
+      <c r="K5" s="59">
         <v>1.1099999999999999E-17</v>
       </c>
       <c r="L5">
@@ -3305,11 +3295,11 @@
       <c r="M5">
         <v>1.6756348498855928E-18</v>
       </c>
-      <c r="N5" s="68">
+      <c r="N5" s="59">
         <f t="shared" si="0"/>
         <v>1.2209999999999999E-14</v>
       </c>
-      <c r="O5" s="70">
+      <c r="O5" s="61">
         <v>1.1099999999999999E-17</v>
       </c>
       <c r="P5">
@@ -3322,17 +3312,17 @@
       </c>
       <c r="T5" s="57"/>
       <c r="U5" s="57"/>
-      <c r="V5" s="70"/>
+      <c r="V5" s="61"/>
       <c r="W5" s="57"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="J6" s="68">
+      <c r="J6" s="59">
         <v>1.2760000000000001E-14</v>
       </c>
-      <c r="K6" s="68">
+      <c r="K6" s="59">
         <v>1.16E-17</v>
       </c>
       <c r="L6">
@@ -3341,11 +3331,11 @@
       <c r="M6">
         <v>1.7511138971777368E-18</v>
       </c>
-      <c r="N6" s="68">
+      <c r="N6" s="59">
         <f t="shared" si="0"/>
         <v>1.2760000000000001E-14</v>
       </c>
-      <c r="O6" s="70">
+      <c r="O6" s="61">
         <v>1.16E-17</v>
       </c>
       <c r="P6">
@@ -3358,17 +3348,17 @@
       </c>
       <c r="T6" s="57"/>
       <c r="U6" s="57"/>
-      <c r="V6" s="70"/>
+      <c r="V6" s="61"/>
       <c r="W6" s="57"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>8</v>
       </c>
-      <c r="J7" s="68">
+      <c r="J7" s="59">
         <v>1.342E-14</v>
       </c>
-      <c r="K7" s="68">
+      <c r="K7" s="59">
         <v>1.22E-17</v>
       </c>
       <c r="L7">
@@ -3377,11 +3367,11 @@
       <c r="M7">
         <v>1.8416887539283094E-18</v>
       </c>
-      <c r="N7" s="68">
+      <c r="N7" s="59">
         <f t="shared" si="0"/>
         <v>1.342E-14</v>
       </c>
-      <c r="O7" s="70">
+      <c r="O7" s="61">
         <v>1.22E-17</v>
       </c>
       <c r="P7">
@@ -3394,17 +3384,17 @@
       </c>
       <c r="T7" s="57"/>
       <c r="U7" s="57"/>
-      <c r="V7" s="70"/>
+      <c r="V7" s="61"/>
       <c r="W7" s="57"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>10</v>
       </c>
-      <c r="J8" s="68">
+      <c r="J8" s="59">
         <v>1.408E-14</v>
       </c>
-      <c r="K8" s="68">
+      <c r="K8" s="59">
         <v>1.28E-17</v>
       </c>
       <c r="L8">
@@ -3413,11 +3403,11 @@
       <c r="M8">
         <v>1.932263610678882E-18</v>
       </c>
-      <c r="N8" s="68">
+      <c r="N8" s="59">
         <f t="shared" si="0"/>
         <v>1.408E-14</v>
       </c>
-      <c r="O8" s="70">
+      <c r="O8" s="61">
         <v>1.28E-17</v>
       </c>
       <c r="P8">
@@ -3430,17 +3420,17 @@
       </c>
       <c r="T8" s="57"/>
       <c r="U8" s="57"/>
-      <c r="V8" s="70"/>
+      <c r="V8" s="61"/>
       <c r="W8" s="57"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>12</v>
       </c>
-      <c r="J9" s="68">
+      <c r="J9" s="59">
         <v>1.4850000000000001E-14</v>
       </c>
-      <c r="K9" s="68">
+      <c r="K9" s="59">
         <v>1.3500000000000001E-17</v>
       </c>
       <c r="L9">
@@ -3449,11 +3439,11 @@
       <c r="M9">
         <v>2.0379342768878833E-18</v>
       </c>
-      <c r="N9" s="68">
+      <c r="N9" s="59">
         <f t="shared" si="0"/>
         <v>1.4850000000000001E-14</v>
       </c>
-      <c r="O9" s="70">
+      <c r="O9" s="61">
         <v>1.3500000000000001E-17</v>
       </c>
       <c r="P9">
@@ -3466,17 +3456,17 @@
       </c>
       <c r="T9" s="57"/>
       <c r="U9" s="57"/>
-      <c r="V9" s="70"/>
+      <c r="V9" s="61"/>
       <c r="W9" s="57"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>14</v>
       </c>
-      <c r="J10" s="68">
+      <c r="J10" s="59">
         <v>1.5620000000000001E-14</v>
       </c>
-      <c r="K10" s="68">
+      <c r="K10" s="59">
         <v>1.4200000000000001E-17</v>
       </c>
       <c r="L10">
@@ -3485,11 +3475,11 @@
       <c r="M10">
         <v>2.1436049430968846E-18</v>
       </c>
-      <c r="N10" s="68">
+      <c r="N10" s="59">
         <f t="shared" si="0"/>
         <v>1.5620000000000001E-14</v>
       </c>
-      <c r="O10" s="70">
+      <c r="O10" s="61">
         <v>1.4200000000000001E-17</v>
       </c>
       <c r="P10">
@@ -3502,17 +3492,17 @@
       </c>
       <c r="T10" s="57"/>
       <c r="U10" s="57"/>
-      <c r="V10" s="70"/>
+      <c r="V10" s="61"/>
       <c r="W10" s="57"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16</v>
       </c>
-      <c r="J11" s="68">
+      <c r="J11" s="59">
         <v>1.639E-14</v>
       </c>
-      <c r="K11" s="68">
+      <c r="K11" s="59">
         <v>1.4899999999999999E-17</v>
       </c>
       <c r="L11">
@@ -3521,11 +3511,11 @@
       <c r="M11">
         <v>2.249275609305886E-18</v>
       </c>
-      <c r="N11" s="68">
+      <c r="N11" s="59">
         <f t="shared" si="0"/>
         <v>1.639E-14</v>
       </c>
-      <c r="O11" s="70">
+      <c r="O11" s="61">
         <v>1.4899999999999999E-17</v>
       </c>
       <c r="P11">
@@ -3538,17 +3528,17 @@
       </c>
       <c r="T11" s="57"/>
       <c r="U11" s="57"/>
-      <c r="V11" s="70"/>
+      <c r="V11" s="61"/>
       <c r="W11" s="57"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>18</v>
       </c>
-      <c r="J12" s="68">
+      <c r="J12" s="59">
         <v>1.7270000000000002E-14</v>
       </c>
-      <c r="K12" s="68">
+      <c r="K12" s="59">
         <v>1.5700000000000001E-17</v>
       </c>
       <c r="L12">
@@ -3557,11 +3547,11 @@
       <c r="M12">
         <v>2.3700420849733161E-18</v>
       </c>
-      <c r="N12" s="68">
+      <c r="N12" s="59">
         <f t="shared" si="0"/>
         <v>1.7270000000000002E-14</v>
       </c>
-      <c r="O12" s="70">
+      <c r="O12" s="61">
         <v>1.5700000000000001E-17</v>
       </c>
       <c r="P12">
@@ -3574,17 +3564,17 @@
       </c>
       <c r="T12" s="57"/>
       <c r="U12" s="57"/>
-      <c r="V12" s="70"/>
+      <c r="V12" s="61"/>
       <c r="W12" s="57"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20</v>
       </c>
-      <c r="J13" s="68">
+      <c r="J13" s="59">
         <v>1.815E-14</v>
       </c>
-      <c r="K13" s="68">
+      <c r="K13" s="59">
         <v>1.65E-17</v>
       </c>
       <c r="L13">
@@ -3593,11 +3583,11 @@
       <c r="M13">
         <v>2.4908085606407462E-18</v>
       </c>
-      <c r="N13" s="68">
+      <c r="N13" s="59">
         <f t="shared" si="0"/>
         <v>1.815E-14</v>
       </c>
-      <c r="O13" s="70">
+      <c r="O13" s="61">
         <v>1.65E-17</v>
       </c>
       <c r="P13">
@@ -3610,17 +3600,17 @@
       </c>
       <c r="T13" s="57"/>
       <c r="U13" s="57"/>
-      <c r="V13" s="70"/>
+      <c r="V13" s="61"/>
       <c r="W13" s="57"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>22</v>
       </c>
-      <c r="J14" s="68">
+      <c r="J14" s="59">
         <v>1.9029999999999999E-14</v>
       </c>
-      <c r="K14" s="68">
+      <c r="K14" s="59">
         <v>1.7299999999999999E-17</v>
       </c>
       <c r="L14">
@@ -3629,11 +3619,11 @@
       <c r="M14">
         <v>2.6115750363081763E-18</v>
       </c>
-      <c r="N14" s="68">
+      <c r="N14" s="59">
         <f t="shared" si="0"/>
         <v>1.9029999999999999E-14</v>
       </c>
-      <c r="O14" s="70">
+      <c r="O14" s="61">
         <v>1.7299999999999999E-17</v>
       </c>
       <c r="P14">
@@ -3646,17 +3636,17 @@
       </c>
       <c r="T14" s="57"/>
       <c r="U14" s="57"/>
-      <c r="V14" s="70"/>
+      <c r="V14" s="61"/>
       <c r="W14" s="57"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>24</v>
       </c>
-      <c r="J15" s="68">
+      <c r="J15" s="59">
         <v>2.002E-14</v>
       </c>
-      <c r="K15" s="68">
+      <c r="K15" s="59">
         <v>1.8199999999999999E-17</v>
       </c>
       <c r="L15">
@@ -3665,11 +3655,11 @@
       <c r="M15">
         <v>2.7474373214340351E-18</v>
       </c>
-      <c r="N15" s="68">
+      <c r="N15" s="59">
         <f t="shared" si="0"/>
         <v>2.002E-14</v>
       </c>
-      <c r="O15" s="70">
+      <c r="O15" s="61">
         <v>1.8199999999999999E-17</v>
       </c>
       <c r="P15">
@@ -3682,17 +3672,17 @@
       </c>
       <c r="T15" s="57"/>
       <c r="U15" s="57"/>
-      <c r="V15" s="70"/>
+      <c r="V15" s="61"/>
       <c r="W15" s="57"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>26</v>
       </c>
-      <c r="J16" s="68">
+      <c r="J16" s="59">
         <v>2.1119999999999999E-14</v>
       </c>
-      <c r="K16" s="68">
+      <c r="K16" s="59">
         <v>1.92E-17</v>
       </c>
       <c r="L16">
@@ -3701,11 +3691,11 @@
       <c r="M16">
         <v>2.8983954160183227E-18</v>
       </c>
-      <c r="N16" s="68">
+      <c r="N16" s="59">
         <f t="shared" si="0"/>
         <v>2.1119999999999999E-14</v>
       </c>
-      <c r="O16" s="70">
+      <c r="O16" s="61">
         <v>1.92E-17</v>
       </c>
       <c r="P16">
@@ -3716,17 +3706,17 @@
         <f t="shared" ref="Q16:Q63" si="2">P16 / density_c</f>
         <v>2.8983954160183227E-18</v>
       </c>
-      <c r="V16" s="70"/>
+      <c r="V16" s="61"/>
       <c r="W16" s="57"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>28</v>
       </c>
-      <c r="J17" s="68">
+      <c r="J17" s="59">
         <v>2.211E-14</v>
       </c>
-      <c r="K17" s="68">
+      <c r="K17" s="59">
         <v>2.0099999999999999E-17</v>
       </c>
       <c r="L17">
@@ -3735,11 +3725,11 @@
       <c r="M17">
         <v>3.0342577011441816E-18</v>
       </c>
-      <c r="N17" s="68">
+      <c r="N17" s="59">
         <f t="shared" si="0"/>
         <v>2.211E-14</v>
       </c>
-      <c r="O17" s="70">
+      <c r="O17" s="61">
         <v>2.0099999999999999E-17</v>
       </c>
       <c r="P17">
@@ -3750,17 +3740,17 @@
         <f t="shared" si="2"/>
         <v>3.0342577011441816E-18</v>
       </c>
-      <c r="V17" s="70"/>
+      <c r="V17" s="61"/>
       <c r="W17" s="57"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>30</v>
       </c>
-      <c r="J18" s="68">
+      <c r="J18" s="59">
         <v>2.3320000000000002E-14</v>
       </c>
-      <c r="K18" s="68">
+      <c r="K18" s="59">
         <v>2.1200000000000001E-17</v>
       </c>
       <c r="L18">
@@ -3769,11 +3759,11 @@
       <c r="M18">
         <v>3.200311605186898E-18</v>
       </c>
-      <c r="N18" s="68">
+      <c r="N18" s="59">
         <f t="shared" si="0"/>
         <v>2.3320000000000002E-14</v>
       </c>
-      <c r="O18" s="70">
+      <c r="O18" s="61">
         <v>2.1200000000000001E-17</v>
       </c>
       <c r="P18">
@@ -3784,17 +3774,17 @@
         <f t="shared" si="2"/>
         <v>3.200311605186898E-18</v>
       </c>
-      <c r="V18" s="70"/>
+      <c r="V18" s="61"/>
       <c r="W18" s="57"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>32</v>
       </c>
-      <c r="J19" s="68">
+      <c r="J19" s="59">
         <v>2.4530000000000001E-14</v>
       </c>
-      <c r="K19" s="68">
+      <c r="K19" s="59">
         <v>2.23E-17</v>
       </c>
       <c r="L19">
@@ -3803,11 +3793,11 @@
       <c r="M19">
         <v>3.3663655092296144E-18</v>
       </c>
-      <c r="N19" s="68">
+      <c r="N19" s="59">
         <f t="shared" si="0"/>
         <v>2.4530000000000001E-14</v>
       </c>
-      <c r="O19" s="70">
+      <c r="O19" s="61">
         <v>2.23E-17</v>
       </c>
       <c r="P19">
@@ -3818,17 +3808,17 @@
         <f t="shared" si="2"/>
         <v>3.3663655092296144E-18</v>
       </c>
-      <c r="V19" s="70"/>
+      <c r="V19" s="61"/>
       <c r="W19" s="57"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>34</v>
       </c>
-      <c r="J20" s="68">
+      <c r="J20" s="59">
         <v>2.5739999999999999E-14</v>
       </c>
-      <c r="K20" s="68">
+      <c r="K20" s="59">
         <v>2.3399999999999999E-17</v>
       </c>
       <c r="L20">
@@ -3837,11 +3827,11 @@
       <c r="M20">
         <v>3.5324194132723304E-18</v>
       </c>
-      <c r="N20" s="68">
+      <c r="N20" s="59">
         <f t="shared" si="0"/>
         <v>2.5739999999999999E-14</v>
       </c>
-      <c r="O20" s="70">
+      <c r="O20" s="61">
         <v>2.3399999999999999E-17</v>
       </c>
       <c r="P20">
@@ -3852,17 +3842,17 @@
         <f t="shared" si="2"/>
         <v>3.5324194132723304E-18</v>
       </c>
-      <c r="V20" s="70"/>
+      <c r="V20" s="61"/>
       <c r="W20" s="57"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>36</v>
       </c>
-      <c r="J21" s="68">
+      <c r="J21" s="59">
         <v>2.7059999999999997E-14</v>
       </c>
-      <c r="K21" s="68">
+      <c r="K21" s="59">
         <v>2.4599999999999999E-17</v>
       </c>
       <c r="L21">
@@ -3871,11 +3861,11 @@
       <c r="M21">
         <v>3.7135691267734763E-18</v>
       </c>
-      <c r="N21" s="68">
+      <c r="N21" s="59">
         <f t="shared" si="0"/>
         <v>2.7059999999999997E-14</v>
       </c>
-      <c r="O21" s="70">
+      <c r="O21" s="61">
         <v>2.4599999999999999E-17</v>
       </c>
       <c r="P21">
@@ -3886,17 +3876,17 @@
         <f t="shared" si="2"/>
         <v>3.7135691267734763E-18</v>
       </c>
-      <c r="V21" s="70"/>
+      <c r="V21" s="61"/>
       <c r="W21" s="57"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>38</v>
       </c>
-      <c r="J22" s="68">
+      <c r="J22" s="59">
         <v>2.849E-14</v>
       </c>
-      <c r="K22" s="68">
+      <c r="K22" s="59">
         <v>2.5899999999999999E-17</v>
       </c>
       <c r="L22">
@@ -3905,11 +3895,11 @@
       <c r="M22">
         <v>3.9098146497330502E-18</v>
       </c>
-      <c r="N22" s="68">
+      <c r="N22" s="59">
         <f t="shared" si="0"/>
         <v>2.849E-14</v>
       </c>
-      <c r="O22" s="70">
+      <c r="O22" s="61">
         <v>2.5899999999999999E-17</v>
       </c>
       <c r="P22">
@@ -3920,17 +3910,17 @@
         <f t="shared" si="2"/>
         <v>3.9098146497330502E-18</v>
       </c>
-      <c r="V22" s="70"/>
+      <c r="V22" s="61"/>
       <c r="W22" s="57"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>40</v>
       </c>
-      <c r="J23" s="68">
+      <c r="J23" s="59">
         <v>2.992E-14</v>
       </c>
-      <c r="K23" s="68">
+      <c r="K23" s="59">
         <v>2.72E-17</v>
       </c>
       <c r="L23">
@@ -3939,11 +3929,11 @@
       <c r="M23">
         <v>4.1060601726926241E-18</v>
       </c>
-      <c r="N23" s="68">
+      <c r="N23" s="59">
         <f t="shared" si="0"/>
         <v>2.992E-14</v>
       </c>
-      <c r="O23" s="70">
+      <c r="O23" s="61">
         <v>2.72E-17</v>
       </c>
       <c r="P23">
@@ -3954,17 +3944,17 @@
         <f t="shared" si="2"/>
         <v>4.1060601726926241E-18</v>
       </c>
-      <c r="V23" s="70"/>
+      <c r="V23" s="61"/>
       <c r="W23" s="57"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>42</v>
       </c>
-      <c r="J24" s="68">
+      <c r="J24" s="59">
         <v>3.1459999999999999E-14</v>
       </c>
-      <c r="K24" s="68">
+      <c r="K24" s="59">
         <v>2.8599999999999999E-17</v>
       </c>
       <c r="L24">
@@ -3973,11 +3963,11 @@
       <c r="M24">
         <v>4.3174015051106268E-18</v>
       </c>
-      <c r="N24" s="68">
+      <c r="N24" s="59">
         <f t="shared" si="0"/>
         <v>3.1459999999999999E-14</v>
       </c>
-      <c r="O24" s="70">
+      <c r="O24" s="61">
         <v>2.8599999999999999E-17</v>
       </c>
       <c r="P24">
@@ -3988,17 +3978,17 @@
         <f t="shared" si="2"/>
         <v>4.3174015051106268E-18</v>
       </c>
-      <c r="V24" s="70"/>
+      <c r="V24" s="61"/>
       <c r="W24" s="57"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>44</v>
       </c>
-      <c r="J25" s="68">
+      <c r="J25" s="59">
         <v>3.2999999999999998E-14</v>
       </c>
-      <c r="K25" s="68">
+      <c r="K25" s="59">
         <v>3.0000000000000001E-17</v>
       </c>
       <c r="L25">
@@ -4007,11 +3997,11 @@
       <c r="M25">
         <v>4.5287428375286295E-18</v>
       </c>
-      <c r="N25" s="68">
+      <c r="N25" s="59">
         <f t="shared" si="0"/>
         <v>3.2999999999999998E-14</v>
       </c>
-      <c r="O25" s="70">
+      <c r="O25" s="61">
         <v>3.0000000000000001E-17</v>
       </c>
       <c r="P25">
@@ -4022,17 +4012,17 @@
         <f t="shared" si="2"/>
         <v>4.5287428375286295E-18</v>
       </c>
-      <c r="V25" s="70"/>
+      <c r="V25" s="61"/>
       <c r="W25" s="57"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>46</v>
       </c>
-      <c r="J26" s="68">
+      <c r="J26" s="59">
         <v>3.4759999999999995E-14</v>
       </c>
-      <c r="K26" s="68">
+      <c r="K26" s="59">
         <v>3.1599999999999998E-17</v>
       </c>
       <c r="L26">
@@ -4041,11 +4031,11 @@
       <c r="M26">
         <v>4.7702757888634897E-18</v>
       </c>
-      <c r="N26" s="68">
+      <c r="N26" s="59">
         <f t="shared" si="0"/>
         <v>3.4759999999999995E-14</v>
       </c>
-      <c r="O26" s="70">
+      <c r="O26" s="61">
         <v>3.1599999999999998E-17</v>
       </c>
       <c r="P26">
@@ -4056,17 +4046,17 @@
         <f t="shared" si="2"/>
         <v>4.7702757888634897E-18</v>
       </c>
-      <c r="V26" s="70"/>
+      <c r="V26" s="61"/>
       <c r="W26" s="57"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>48</v>
       </c>
-      <c r="J27" s="68">
+      <c r="J27" s="59">
         <v>3.6520000000000005E-14</v>
       </c>
-      <c r="K27" s="68">
+      <c r="K27" s="59">
         <v>3.3200000000000002E-17</v>
       </c>
       <c r="L27">
@@ -4075,11 +4065,11 @@
       <c r="M27">
         <v>5.0118087401983498E-18</v>
       </c>
-      <c r="N27" s="68">
+      <c r="N27" s="59">
         <f t="shared" si="0"/>
         <v>3.6520000000000005E-14</v>
       </c>
-      <c r="O27" s="70">
+      <c r="O27" s="61">
         <v>3.3200000000000002E-17</v>
       </c>
       <c r="P27">
@@ -4090,17 +4080,17 @@
         <f t="shared" si="2"/>
         <v>5.0118087401983498E-18</v>
       </c>
-      <c r="V27" s="70"/>
+      <c r="V27" s="61"/>
       <c r="W27" s="57"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>50</v>
       </c>
-      <c r="J28" s="68">
+      <c r="J28" s="59">
         <v>3.8389999999999995E-14</v>
       </c>
-      <c r="K28" s="68">
+      <c r="K28" s="59">
         <v>3.4899999999999998E-17</v>
       </c>
       <c r="L28">
@@ -4109,11 +4099,11 @@
       <c r="M28">
         <v>5.2684375009916388E-18</v>
       </c>
-      <c r="N28" s="68">
+      <c r="N28" s="59">
         <f t="shared" si="0"/>
         <v>3.8389999999999995E-14</v>
       </c>
-      <c r="O28" s="70">
+      <c r="O28" s="61">
         <v>3.4899999999999998E-17</v>
       </c>
       <c r="P28">
@@ -4124,17 +4114,17 @@
         <f t="shared" si="2"/>
         <v>5.2684375009916388E-18</v>
       </c>
-      <c r="V28" s="70"/>
+      <c r="V28" s="61"/>
       <c r="W28" s="57"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>52</v>
       </c>
-      <c r="J29" s="68">
+      <c r="J29" s="59">
         <v>4.0369999999999996E-14</v>
       </c>
-      <c r="K29" s="68">
+      <c r="K29" s="59">
         <v>3.6699999999999997E-17</v>
       </c>
       <c r="L29">
@@ -4143,11 +4133,11 @@
       <c r="M29">
         <v>5.5401620712433565E-18</v>
       </c>
-      <c r="N29" s="68">
+      <c r="N29" s="59">
         <f t="shared" si="0"/>
         <v>4.0369999999999996E-14</v>
       </c>
-      <c r="O29" s="70">
+      <c r="O29" s="61">
         <v>3.6699999999999997E-17</v>
       </c>
       <c r="P29">
@@ -4158,17 +4148,17 @@
         <f t="shared" si="2"/>
         <v>5.5401620712433565E-18</v>
       </c>
-      <c r="V29" s="70"/>
+      <c r="V29" s="61"/>
       <c r="W29" s="57"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>54</v>
       </c>
-      <c r="J30" s="68">
+      <c r="J30" s="59">
         <v>4.2460000000000003E-14</v>
       </c>
-      <c r="K30" s="68">
+      <c r="K30" s="59">
         <v>3.8600000000000001E-17</v>
       </c>
       <c r="L30">
@@ -4177,11 +4167,11 @@
       <c r="M30">
         <v>5.826982450953503E-18</v>
       </c>
-      <c r="N30" s="68">
+      <c r="N30" s="59">
         <f t="shared" si="0"/>
         <v>4.2460000000000003E-14</v>
       </c>
-      <c r="O30" s="70">
+      <c r="O30" s="61">
         <v>3.8600000000000001E-17</v>
       </c>
       <c r="P30">
@@ -4192,17 +4182,17 @@
         <f t="shared" si="2"/>
         <v>5.826982450953503E-18</v>
       </c>
-      <c r="V30" s="70"/>
+      <c r="V30" s="61"/>
       <c r="W30" s="57"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>56</v>
       </c>
-      <c r="J31" s="68">
+      <c r="J31" s="59">
         <v>4.4660000000000002E-14</v>
       </c>
-      <c r="K31" s="68">
+      <c r="K31" s="59">
         <v>4.0600000000000003E-17</v>
       </c>
       <c r="L31">
@@ -4211,11 +4201,11 @@
       <c r="M31">
         <v>6.1288986401220783E-18</v>
       </c>
-      <c r="N31" s="68">
+      <c r="N31" s="59">
         <f t="shared" si="0"/>
         <v>4.4660000000000002E-14</v>
       </c>
-      <c r="O31" s="70">
+      <c r="O31" s="61">
         <v>4.0600000000000003E-17</v>
       </c>
       <c r="P31">
@@ -4226,17 +4216,17 @@
         <f t="shared" si="2"/>
         <v>6.1288986401220783E-18</v>
       </c>
-      <c r="V31" s="70"/>
+      <c r="V31" s="61"/>
       <c r="W31" s="57"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>58</v>
       </c>
-      <c r="J32" s="68">
+      <c r="J32" s="59">
         <v>4.6859999999999995E-14</v>
       </c>
-      <c r="K32" s="68">
+      <c r="K32" s="59">
         <v>4.2599999999999998E-17</v>
       </c>
       <c r="L32">
@@ -4245,11 +4235,11 @@
       <c r="M32">
         <v>6.4308148292906535E-18</v>
       </c>
-      <c r="N32" s="68">
+      <c r="N32" s="59">
         <f t="shared" si="0"/>
         <v>4.6859999999999995E-14</v>
       </c>
-      <c r="O32" s="70">
+      <c r="O32" s="61">
         <v>4.2599999999999998E-17</v>
       </c>
       <c r="P32">
@@ -4260,17 +4250,17 @@
         <f t="shared" si="2"/>
         <v>6.4308148292906535E-18</v>
       </c>
-      <c r="V32" s="70"/>
+      <c r="V32" s="61"/>
       <c r="W32" s="57"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>60</v>
       </c>
-      <c r="J33" s="68">
+      <c r="J33" s="59">
         <v>4.9279999999999999E-14</v>
       </c>
-      <c r="K33" s="68">
+      <c r="K33" s="59">
         <v>4.4800000000000002E-17</v>
       </c>
       <c r="L33">
@@ -4279,11 +4269,11 @@
       <c r="M33">
         <v>6.7629226373760863E-18</v>
       </c>
-      <c r="N33" s="68">
+      <c r="N33" s="59">
         <f t="shared" si="0"/>
         <v>4.9279999999999999E-14</v>
       </c>
-      <c r="O33" s="70">
+      <c r="O33" s="61">
         <v>4.4800000000000002E-17</v>
       </c>
       <c r="P33">
@@ -4294,17 +4284,17 @@
         <f t="shared" si="2"/>
         <v>6.7629226373760863E-18</v>
       </c>
-      <c r="V33" s="70"/>
+      <c r="V33" s="61"/>
       <c r="W33" s="57"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>62</v>
       </c>
-      <c r="J34" s="68">
+      <c r="J34" s="59">
         <v>5.1809999999999996E-14</v>
       </c>
-      <c r="K34" s="68">
+      <c r="K34" s="59">
         <v>4.7099999999999997E-17</v>
       </c>
       <c r="L34">
@@ -4313,11 +4303,11 @@
       <c r="M34">
         <v>7.1101262549199486E-18</v>
       </c>
-      <c r="N34" s="68">
+      <c r="N34" s="59">
         <f t="shared" si="0"/>
         <v>5.1809999999999996E-14</v>
       </c>
-      <c r="O34" s="70">
+      <c r="O34" s="61">
         <v>4.7099999999999997E-17</v>
       </c>
       <c r="P34">
@@ -4328,17 +4318,17 @@
         <f t="shared" si="2"/>
         <v>7.1101262549199486E-18</v>
       </c>
-      <c r="V34" s="70"/>
+      <c r="V34" s="61"/>
       <c r="W34" s="57"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>64</v>
       </c>
-      <c r="J35" s="68">
+      <c r="J35" s="59">
         <v>5.4449999999999998E-14</v>
       </c>
-      <c r="K35" s="68">
+      <c r="K35" s="59">
         <v>4.9499999999999997E-17</v>
       </c>
       <c r="L35">
@@ -4347,11 +4337,11 @@
       <c r="M35">
         <v>7.4724256819222389E-18</v>
       </c>
-      <c r="N35" s="68">
+      <c r="N35" s="59">
         <f t="shared" si="0"/>
         <v>5.4449999999999998E-14</v>
       </c>
-      <c r="O35" s="70">
+      <c r="O35" s="61">
         <v>4.9499999999999997E-17</v>
       </c>
       <c r="P35">
@@ -4362,17 +4352,17 @@
         <f t="shared" si="2"/>
         <v>7.4724256819222389E-18</v>
       </c>
-      <c r="V35" s="70"/>
+      <c r="V35" s="61"/>
       <c r="W35" s="57"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>66</v>
       </c>
-      <c r="J36" s="68">
+      <c r="J36" s="59">
         <v>5.7309999999999998E-14</v>
       </c>
-      <c r="K36" s="68">
+      <c r="K36" s="59">
         <v>5.2099999999999999E-17</v>
       </c>
       <c r="L36">
@@ -4381,11 +4371,11 @@
       <c r="M36">
         <v>7.8649167278413852E-18</v>
       </c>
-      <c r="N36" s="68">
+      <c r="N36" s="59">
         <f t="shared" si="0"/>
         <v>5.7309999999999998E-14</v>
       </c>
-      <c r="O36" s="70">
+      <c r="O36" s="61">
         <v>5.2099999999999999E-17</v>
       </c>
       <c r="P36">
@@ -4396,17 +4386,17 @@
         <f t="shared" si="2"/>
         <v>7.8649167278413852E-18</v>
       </c>
-      <c r="V36" s="70"/>
+      <c r="V36" s="61"/>
       <c r="W36" s="57"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>68</v>
       </c>
-      <c r="J37" s="68">
+      <c r="J37" s="59">
         <v>6.0169999999999998E-14</v>
       </c>
-      <c r="K37" s="68">
+      <c r="K37" s="59">
         <v>5.47E-17</v>
       </c>
       <c r="L37">
@@ -4415,11 +4405,11 @@
       <c r="M37">
         <v>8.2574077737605345E-18</v>
       </c>
-      <c r="N37" s="68">
+      <c r="N37" s="59">
         <f t="shared" si="0"/>
         <v>6.0169999999999998E-14</v>
       </c>
-      <c r="O37" s="70">
+      <c r="O37" s="61">
         <v>5.47E-17</v>
       </c>
       <c r="P37">
@@ -4430,17 +4420,17 @@
         <f t="shared" si="2"/>
         <v>8.2574077737605345E-18</v>
       </c>
-      <c r="V37" s="70"/>
+      <c r="V37" s="61"/>
       <c r="W37" s="57"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>70</v>
       </c>
-      <c r="J38" s="68">
+      <c r="J38" s="59">
         <v>6.3249999999999996E-14</v>
       </c>
-      <c r="K38" s="68">
+      <c r="K38" s="59">
         <v>5.7499999999999998E-17</v>
       </c>
       <c r="L38">
@@ -4449,11 +4439,11 @@
       <c r="M38">
         <v>8.6800904385965399E-18</v>
       </c>
-      <c r="N38" s="68">
+      <c r="N38" s="59">
         <f t="shared" si="0"/>
         <v>6.3249999999999996E-14</v>
       </c>
-      <c r="O38" s="70">
+      <c r="O38" s="61">
         <v>5.7499999999999998E-17</v>
       </c>
       <c r="P38">
@@ -4464,17 +4454,17 @@
         <f t="shared" si="2"/>
         <v>8.6800904385965399E-18</v>
       </c>
-      <c r="V38" s="70"/>
+      <c r="V38" s="61"/>
       <c r="W38" s="57"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>72</v>
       </c>
-      <c r="J39" s="68">
+      <c r="J39" s="59">
         <v>6.6549999999999992E-14</v>
       </c>
-      <c r="K39" s="68">
+      <c r="K39" s="59">
         <v>6.0499999999999997E-17</v>
       </c>
       <c r="L39">
@@ -4483,11 +4473,11 @@
       <c r="M39">
         <v>9.1329647223494027E-18</v>
       </c>
-      <c r="N39" s="68">
+      <c r="N39" s="59">
         <f t="shared" si="0"/>
         <v>6.6549999999999992E-14</v>
       </c>
-      <c r="O39" s="70">
+      <c r="O39" s="61">
         <v>6.0499999999999997E-17</v>
       </c>
       <c r="P39">
@@ -4498,17 +4488,17 @@
         <f t="shared" si="2"/>
         <v>9.1329647223494027E-18</v>
       </c>
-      <c r="V39" s="70"/>
+      <c r="V39" s="61"/>
       <c r="W39" s="57"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>74</v>
       </c>
-      <c r="J40" s="68">
+      <c r="J40" s="59">
         <v>6.9959999999999999E-14</v>
       </c>
-      <c r="K40" s="68">
+      <c r="K40" s="59">
         <v>6.3600000000000001E-17</v>
       </c>
       <c r="L40">
@@ -4517,11 +4507,11 @@
       <c r="M40">
         <v>9.6009348155606944E-18</v>
       </c>
-      <c r="N40" s="68">
+      <c r="N40" s="59">
         <f t="shared" si="0"/>
         <v>6.9959999999999999E-14</v>
       </c>
-      <c r="O40" s="70">
+      <c r="O40" s="61">
         <v>6.3600000000000001E-17</v>
       </c>
       <c r="P40">
@@ -4532,17 +4522,17 @@
         <f t="shared" si="2"/>
         <v>9.6009348155606944E-18</v>
       </c>
-      <c r="V40" s="70"/>
+      <c r="V40" s="61"/>
       <c r="W40" s="57"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>76</v>
       </c>
-      <c r="J41" s="68">
+      <c r="J41" s="59">
         <v>7.3590000000000005E-14</v>
       </c>
-      <c r="K41" s="68">
+      <c r="K41" s="59">
         <v>6.69E-17</v>
       </c>
       <c r="L41">
@@ -4551,11 +4541,11 @@
       <c r="M41">
         <v>1.0099096527688844E-17</v>
       </c>
-      <c r="N41" s="68">
+      <c r="N41" s="59">
         <f t="shared" si="0"/>
         <v>7.3590000000000005E-14</v>
       </c>
-      <c r="O41" s="70">
+      <c r="O41" s="61">
         <v>6.69E-17</v>
       </c>
       <c r="P41">
@@ -4566,17 +4556,17 @@
         <f t="shared" si="2"/>
         <v>1.0099096527688844E-17</v>
       </c>
-      <c r="V41" s="70"/>
+      <c r="V41" s="61"/>
       <c r="W41" s="57"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>78</v>
       </c>
-      <c r="J42" s="68">
+      <c r="J42" s="59">
         <v>7.733000000000001E-14</v>
       </c>
-      <c r="K42" s="68">
+      <c r="K42" s="59">
         <v>7.0300000000000003E-17</v>
       </c>
       <c r="L42">
@@ -4585,11 +4575,11 @@
       <c r="M42">
         <v>1.0612354049275421E-17</v>
       </c>
-      <c r="N42" s="68">
+      <c r="N42" s="59">
         <f t="shared" si="0"/>
         <v>7.733000000000001E-14</v>
       </c>
-      <c r="O42" s="70">
+      <c r="O42" s="61">
         <v>7.0300000000000003E-17</v>
       </c>
       <c r="P42">
@@ -4600,17 +4590,17 @@
         <f t="shared" si="2"/>
         <v>1.0612354049275421E-17</v>
       </c>
-      <c r="V42" s="70"/>
+      <c r="V42" s="61"/>
       <c r="W42" s="57"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>80</v>
       </c>
-      <c r="J43" s="68">
+      <c r="J43" s="59">
         <v>8.129E-14</v>
       </c>
-      <c r="K43" s="68">
+      <c r="K43" s="59">
         <v>7.3900000000000003E-17</v>
       </c>
       <c r="L43">
@@ -4619,11 +4609,11 @@
       <c r="M43">
         <v>1.1155803189778857E-17</v>
       </c>
-      <c r="N43" s="68">
+      <c r="N43" s="59">
         <f t="shared" si="0"/>
         <v>8.129E-14</v>
       </c>
-      <c r="O43" s="70">
+      <c r="O43" s="61">
         <v>7.3900000000000003E-17</v>
       </c>
       <c r="P43">
@@ -4634,17 +4624,17 @@
         <f t="shared" si="2"/>
         <v>1.1155803189778857E-17</v>
       </c>
-      <c r="V43" s="70"/>
+      <c r="V43" s="61"/>
       <c r="W43" s="57"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>82</v>
       </c>
-      <c r="J44" s="68">
+      <c r="J44" s="59">
         <v>8.5470000000000001E-14</v>
       </c>
-      <c r="K44" s="68">
+      <c r="K44" s="59">
         <v>7.7699999999999998E-17</v>
       </c>
       <c r="L44">
@@ -4653,11 +4643,11 @@
       <c r="M44">
         <v>1.172944394919915E-17</v>
       </c>
-      <c r="N44" s="68">
+      <c r="N44" s="59">
         <f t="shared" si="0"/>
         <v>8.5470000000000001E-14</v>
       </c>
-      <c r="O44" s="70">
+      <c r="O44" s="61">
         <v>7.7699999999999998E-17</v>
       </c>
       <c r="P44">
@@ -4668,17 +4658,17 @@
         <f t="shared" si="2"/>
         <v>1.172944394919915E-17</v>
       </c>
-      <c r="V44" s="70"/>
+      <c r="V44" s="61"/>
       <c r="W44" s="57"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>84</v>
       </c>
-      <c r="J45" s="68">
+      <c r="J45" s="59">
         <v>8.987E-14</v>
       </c>
-      <c r="K45" s="68">
+      <c r="K45" s="59">
         <v>8.1700000000000001E-17</v>
       </c>
       <c r="L45">
@@ -4687,11 +4677,11 @@
       <c r="M45">
         <v>1.23332763275363E-17</v>
       </c>
-      <c r="N45" s="68">
+      <c r="N45" s="59">
         <f t="shared" si="0"/>
         <v>8.987E-14</v>
       </c>
-      <c r="O45" s="70">
+      <c r="O45" s="61">
         <v>8.1700000000000001E-17</v>
       </c>
       <c r="P45">
@@ -4702,17 +4692,17 @@
         <f t="shared" si="2"/>
         <v>1.23332763275363E-17</v>
       </c>
-      <c r="V45" s="70"/>
+      <c r="V45" s="61"/>
       <c r="W45" s="57"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>86</v>
       </c>
-      <c r="J46" s="68">
+      <c r="J46" s="59">
         <v>9.4379999999999998E-14</v>
       </c>
-      <c r="K46" s="68">
+      <c r="K46" s="59">
         <v>8.5799999999999996E-17</v>
       </c>
       <c r="L46">
@@ -4721,11 +4711,11 @@
       <c r="M46">
         <v>1.295220451533188E-17</v>
       </c>
-      <c r="N46" s="68">
+      <c r="N46" s="59">
         <f t="shared" si="0"/>
         <v>9.4379999999999998E-14</v>
       </c>
-      <c r="O46" s="70">
+      <c r="O46" s="61">
         <v>8.5799999999999996E-17</v>
       </c>
       <c r="P46">
@@ -4736,17 +4726,17 @@
         <f t="shared" si="2"/>
         <v>1.295220451533188E-17</v>
       </c>
-      <c r="V46" s="70"/>
+      <c r="V46" s="61"/>
       <c r="W46" s="57"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>88</v>
       </c>
-      <c r="J47" s="68">
+      <c r="J47" s="59">
         <v>9.9220000000000005E-14</v>
       </c>
-      <c r="K47" s="68">
+      <c r="K47" s="59">
         <v>9.0200000000000004E-17</v>
       </c>
       <c r="L47">
@@ -4755,11 +4745,11 @@
       <c r="M47">
         <v>1.3616420131502747E-17</v>
       </c>
-      <c r="N47" s="68">
+      <c r="N47" s="59">
         <f t="shared" si="0"/>
         <v>9.9220000000000005E-14</v>
       </c>
-      <c r="O47" s="70">
+      <c r="O47" s="61">
         <v>9.0200000000000004E-17</v>
       </c>
       <c r="P47">
@@ -4770,17 +4760,17 @@
         <f t="shared" si="2"/>
         <v>1.3616420131502747E-17</v>
       </c>
-      <c r="V47" s="70"/>
+      <c r="V47" s="61"/>
       <c r="W47" s="57"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>90</v>
       </c>
-      <c r="J48" s="68">
+      <c r="J48" s="59">
         <v>1.0439E-13</v>
       </c>
-      <c r="K48" s="68">
+      <c r="K48" s="59">
         <v>9.4899999999999999E-17</v>
       </c>
       <c r="L48">
@@ -4789,11 +4779,11 @@
       <c r="M48">
         <v>1.4325923176048897E-17</v>
       </c>
-      <c r="N48" s="68">
+      <c r="N48" s="59">
         <f t="shared" si="0"/>
         <v>1.0439E-13</v>
       </c>
-      <c r="O48" s="70">
+      <c r="O48" s="61">
         <v>9.4899999999999999E-17</v>
       </c>
       <c r="P48">
@@ -4804,17 +4794,17 @@
         <f t="shared" si="2"/>
         <v>1.4325923176048897E-17</v>
       </c>
-      <c r="V48" s="70"/>
+      <c r="V48" s="61"/>
       <c r="W48" s="57"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>92</v>
       </c>
-      <c r="J49" s="68">
+      <c r="J49" s="59">
         <v>1.0967E-13</v>
       </c>
-      <c r="K49" s="68">
+      <c r="K49" s="59">
         <v>9.9699999999999998E-17</v>
       </c>
       <c r="L49">
@@ -4823,11 +4813,11 @@
       <c r="M49">
         <v>1.5050522030053478E-17</v>
       </c>
-      <c r="N49" s="68">
+      <c r="N49" s="59">
         <f t="shared" si="0"/>
         <v>1.0967E-13</v>
       </c>
-      <c r="O49" s="70">
+      <c r="O49" s="61">
         <v>9.9699999999999998E-17</v>
       </c>
       <c r="P49">
@@ -4838,17 +4828,17 @@
         <f t="shared" si="2"/>
         <v>1.5050522030053478E-17</v>
       </c>
-      <c r="V49" s="70"/>
+      <c r="V49" s="61"/>
       <c r="W49" s="57"/>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>94</v>
       </c>
-      <c r="J50" s="68">
+      <c r="J50" s="59">
         <v>1.1539E-13</v>
       </c>
-      <c r="K50" s="68">
+      <c r="K50" s="59">
         <v>1.049E-16</v>
       </c>
       <c r="L50">
@@ -4857,11 +4847,11 @@
       <c r="M50">
         <v>1.5835504121891776E-17</v>
       </c>
-      <c r="N50" s="68">
+      <c r="N50" s="59">
         <f t="shared" si="0"/>
         <v>1.1539E-13</v>
       </c>
-      <c r="O50" s="70">
+      <c r="O50" s="61">
         <v>1.049E-16</v>
       </c>
       <c r="P50">
@@ -4872,17 +4862,17 @@
         <f t="shared" si="2"/>
         <v>1.5835504121891776E-17</v>
       </c>
-      <c r="V50" s="70"/>
+      <c r="V50" s="61"/>
       <c r="W50" s="57"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>96</v>
       </c>
-      <c r="J51" s="68">
+      <c r="J51" s="59">
         <v>1.2121999999999999E-13</v>
       </c>
-      <c r="K51" s="68">
+      <c r="K51" s="59">
         <v>1.102E-16</v>
       </c>
       <c r="L51">
@@ -4891,11 +4881,11 @@
       <c r="M51">
         <v>1.6635582023188499E-17</v>
       </c>
-      <c r="N51" s="68">
+      <c r="N51" s="59">
         <f t="shared" si="0"/>
         <v>1.2121999999999999E-13</v>
       </c>
-      <c r="O51" s="70">
+      <c r="O51" s="61">
         <v>1.102E-16</v>
       </c>
       <c r="P51">
@@ -4906,17 +4896,17 @@
         <f t="shared" si="2"/>
         <v>1.6635582023188499E-17</v>
       </c>
-      <c r="V51" s="70"/>
+      <c r="V51" s="61"/>
       <c r="W51" s="57"/>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>98</v>
       </c>
-      <c r="J52" s="68">
+      <c r="J52" s="59">
         <v>1.2748999999999999E-13</v>
       </c>
-      <c r="K52" s="68">
+      <c r="K52" s="59">
         <v>1.1589999999999999E-16</v>
       </c>
       <c r="L52">
@@ -4925,11 +4915,11 @@
       <c r="M52">
         <v>1.7496043162318937E-17</v>
       </c>
-      <c r="N52" s="68">
+      <c r="N52" s="59">
         <f t="shared" si="0"/>
         <v>1.2748999999999999E-13</v>
       </c>
-      <c r="O52" s="70">
+      <c r="O52" s="61">
         <v>1.1589999999999999E-16</v>
       </c>
       <c r="P52">
@@ -4940,17 +4930,17 @@
         <f t="shared" si="2"/>
         <v>1.7496043162318937E-17</v>
       </c>
-      <c r="V52" s="70"/>
+      <c r="V52" s="61"/>
       <c r="W52" s="57"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>100</v>
       </c>
-      <c r="J53" s="68">
+      <c r="J53" s="59">
         <v>1.3398E-13</v>
       </c>
-      <c r="K53" s="68">
+      <c r="K53" s="59">
         <v>1.218E-16</v>
       </c>
       <c r="L53">
@@ -4959,11 +4949,11 @@
       <c r="M53">
         <v>1.8386695920366236E-17</v>
       </c>
-      <c r="N53" s="68">
+      <c r="N53" s="59">
         <f t="shared" si="0"/>
         <v>1.3398E-13</v>
       </c>
-      <c r="O53" s="70">
+      <c r="O53" s="61">
         <v>1.218E-16</v>
       </c>
       <c r="P53">
@@ -4974,17 +4964,17 @@
         <f t="shared" si="2"/>
         <v>1.8386695920366236E-17</v>
       </c>
-      <c r="V53" s="70"/>
+      <c r="V53" s="61"/>
       <c r="W53" s="57"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>102</v>
       </c>
-      <c r="J54" s="68">
+      <c r="J54" s="59">
         <v>1.4091E-13</v>
       </c>
-      <c r="K54" s="68">
+      <c r="K54" s="59">
         <v>1.281E-16</v>
       </c>
       <c r="L54">
@@ -4993,11 +4983,11 @@
       <c r="M54">
         <v>1.9337731916247246E-17</v>
       </c>
-      <c r="N54" s="68">
+      <c r="N54" s="59">
         <f t="shared" si="0"/>
         <v>1.4091E-13</v>
       </c>
-      <c r="O54" s="70">
+      <c r="O54" s="61">
         <v>1.281E-16</v>
       </c>
       <c r="P54">
@@ -5008,17 +4998,17 @@
         <f t="shared" si="2"/>
         <v>1.9337731916247246E-17</v>
       </c>
-      <c r="V54" s="70"/>
+      <c r="V54" s="61"/>
       <c r="W54" s="57"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>104</v>
       </c>
-      <c r="J55" s="68">
+      <c r="J55" s="59">
         <v>1.4806E-13</v>
       </c>
-      <c r="K55" s="68">
+      <c r="K55" s="59">
         <v>1.3460000000000001E-16</v>
       </c>
       <c r="L55">
@@ -5027,11 +5017,11 @@
       <c r="M55">
         <v>2.031895953104512E-17</v>
       </c>
-      <c r="N55" s="68">
+      <c r="N55" s="59">
         <f t="shared" si="0"/>
         <v>1.4806E-13</v>
       </c>
-      <c r="O55" s="70">
+      <c r="O55" s="61">
         <v>1.3460000000000001E-16</v>
       </c>
       <c r="P55">
@@ -5042,17 +5032,17 @@
         <f t="shared" si="2"/>
         <v>2.031895953104512E-17</v>
       </c>
-      <c r="V55" s="70"/>
+      <c r="V55" s="61"/>
       <c r="W55" s="57"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>106</v>
       </c>
-      <c r="J56" s="68">
+      <c r="J56" s="59">
         <v>1.5565E-13</v>
       </c>
-      <c r="K56" s="68">
+      <c r="K56" s="59">
         <v>1.4150000000000001E-16</v>
       </c>
       <c r="L56">
@@ -5061,11 +5051,11 @@
       <c r="M56">
         <v>2.1360570383676703E-17</v>
       </c>
-      <c r="N56" s="68">
+      <c r="N56" s="59">
         <f t="shared" si="0"/>
         <v>1.5565E-13</v>
       </c>
-      <c r="O56" s="70">
+      <c r="O56" s="61">
         <v>1.4150000000000001E-16</v>
       </c>
       <c r="P56">
@@ -5076,17 +5066,17 @@
         <f t="shared" si="2"/>
         <v>2.1360570383676703E-17</v>
       </c>
-      <c r="V56" s="70"/>
+      <c r="V56" s="61"/>
       <c r="W56" s="57"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>108</v>
       </c>
-      <c r="J57" s="68">
+      <c r="J57" s="59">
         <v>1.6367999999999999E-13</v>
       </c>
-      <c r="K57" s="68">
+      <c r="K57" s="59">
         <v>1.488E-16</v>
       </c>
       <c r="L57">
@@ -5095,11 +5085,11 @@
       <c r="M57">
         <v>2.2462564474142001E-17</v>
       </c>
-      <c r="N57" s="68">
+      <c r="N57" s="59">
         <f t="shared" si="0"/>
         <v>1.6367999999999999E-13</v>
       </c>
-      <c r="O57" s="70">
+      <c r="O57" s="61">
         <v>1.488E-16</v>
       </c>
       <c r="P57">
@@ -5110,17 +5100,17 @@
         <f t="shared" si="2"/>
         <v>2.2462564474142001E-17</v>
       </c>
-      <c r="V57" s="70"/>
+      <c r="V57" s="61"/>
       <c r="W57" s="57"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>110</v>
       </c>
-      <c r="J58" s="68">
+      <c r="J58" s="59">
         <v>1.7204000000000002E-13</v>
       </c>
-      <c r="K58" s="68">
+      <c r="K58" s="59">
         <v>1.5640000000000001E-16</v>
       </c>
       <c r="L58">
@@ -5129,11 +5119,11 @@
       <c r="M58">
         <v>2.3609845992982587E-17</v>
       </c>
-      <c r="N58" s="68">
+      <c r="N58" s="59">
         <f t="shared" si="0"/>
         <v>1.7204000000000002E-13</v>
       </c>
-      <c r="O58" s="70">
+      <c r="O58" s="61">
         <v>1.5640000000000001E-16</v>
       </c>
       <c r="P58">
@@ -5144,17 +5134,17 @@
         <f t="shared" si="2"/>
         <v>2.3609845992982587E-17</v>
       </c>
-      <c r="V58" s="70"/>
+      <c r="V58" s="61"/>
       <c r="W58" s="57"/>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>112</v>
       </c>
-      <c r="J59" s="68">
+      <c r="J59" s="59">
         <v>1.8083999999999999E-13</v>
       </c>
-      <c r="K59" s="68">
+      <c r="K59" s="59">
         <v>1.6439999999999999E-16</v>
       </c>
       <c r="L59">
@@ -5163,11 +5153,11 @@
       <c r="M59">
         <v>2.4817510749656888E-17</v>
       </c>
-      <c r="N59" s="68">
+      <c r="N59" s="59">
         <f t="shared" si="0"/>
         <v>1.8083999999999999E-13</v>
       </c>
-      <c r="O59" s="70">
+      <c r="O59" s="61">
         <v>1.6439999999999999E-16</v>
       </c>
       <c r="P59">
@@ -5178,17 +5168,17 @@
         <f t="shared" si="2"/>
         <v>2.4817510749656888E-17</v>
       </c>
-      <c r="V59" s="70"/>
+      <c r="V59" s="61"/>
       <c r="W59" s="57"/>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>114</v>
       </c>
-      <c r="J60" s="68">
+      <c r="J60" s="59">
         <v>1.9019000000000002E-13</v>
       </c>
-      <c r="K60" s="68">
+      <c r="K60" s="59">
         <v>1.7290000000000001E-16</v>
       </c>
       <c r="L60">
@@ -5197,11 +5187,11 @@
       <c r="M60">
         <v>2.6100654553623335E-17</v>
       </c>
-      <c r="N60" s="68">
+      <c r="N60" s="59">
         <f t="shared" si="0"/>
         <v>1.9019000000000002E-13</v>
       </c>
-      <c r="O60" s="70">
+      <c r="O60" s="61">
         <v>1.7290000000000001E-16</v>
       </c>
       <c r="P60">
@@ -5212,17 +5202,17 @@
         <f t="shared" si="2"/>
         <v>2.6100654553623335E-17</v>
       </c>
-      <c r="V60" s="70"/>
+      <c r="V60" s="61"/>
       <c r="W60" s="57"/>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>116</v>
       </c>
-      <c r="J61" s="68">
+      <c r="J61" s="59">
         <v>1.9987000000000001E-13</v>
       </c>
-      <c r="K61" s="68">
+      <c r="K61" s="59">
         <v>1.817E-16</v>
       </c>
       <c r="L61">
@@ -5231,11 +5221,11 @@
       <c r="M61">
         <v>2.7429085785965066E-17</v>
       </c>
-      <c r="N61" s="68">
+      <c r="N61" s="59">
         <f t="shared" si="0"/>
         <v>1.9987000000000001E-13</v>
       </c>
-      <c r="O61" s="70">
+      <c r="O61" s="61">
         <v>1.817E-16</v>
       </c>
       <c r="P61">
@@ -5246,17 +5236,17 @@
         <f t="shared" si="2"/>
         <v>2.7429085785965066E-17</v>
       </c>
-      <c r="V61" s="70"/>
+      <c r="V61" s="61"/>
       <c r="W61" s="57"/>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>118</v>
       </c>
-      <c r="J62" s="68">
+      <c r="J62" s="59">
         <v>2.1020999999999999E-13</v>
       </c>
-      <c r="K62" s="68">
+      <c r="K62" s="59">
         <v>1.9109999999999999E-16</v>
       </c>
       <c r="L62">
@@ -5265,11 +5255,11 @@
       <c r="M62">
         <v>2.8848091875057372E-17</v>
       </c>
-      <c r="N62" s="68">
+      <c r="N62" s="59">
         <f t="shared" si="0"/>
         <v>2.1020999999999999E-13</v>
       </c>
-      <c r="O62" s="70">
+      <c r="O62" s="61">
         <v>1.9109999999999999E-16</v>
       </c>
       <c r="P62">
@@ -5280,17 +5270,17 @@
         <f t="shared" si="2"/>
         <v>2.8848091875057372E-17</v>
       </c>
-      <c r="V62" s="70"/>
+      <c r="V62" s="61"/>
       <c r="W62" s="57"/>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>120</v>
       </c>
-      <c r="J63" s="68">
+      <c r="J63" s="59">
         <v>2.2099E-13</v>
       </c>
-      <c r="K63" s="68">
+      <c r="K63" s="59">
         <v>2.009E-16</v>
       </c>
       <c r="L63">
@@ -5299,11 +5289,11 @@
       <c r="M63">
         <v>3.0327481201983388E-17</v>
       </c>
-      <c r="N63" s="68">
+      <c r="N63" s="59">
         <f t="shared" si="0"/>
         <v>2.2099E-13</v>
       </c>
-      <c r="O63" s="70">
+      <c r="O63" s="61">
         <v>2.009E-16</v>
       </c>
       <c r="P63">
@@ -5314,7 +5304,7 @@
         <f t="shared" si="2"/>
         <v>3.0327481201983388E-17</v>
       </c>
-      <c r="V63" s="70"/>
+      <c r="V63" s="61"/>
       <c r="W63" s="57"/>
     </row>
   </sheetData>
@@ -5326,10 +5316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5382,10 +5369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5482,10 +5466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
-    </sheetView>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -5522,11 +5503,11 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -7639,10 +7620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -7732,10 +7710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7798,10 +7773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7861,8 +7833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7927,10 +7898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -8028,7 +7996,7 @@
       </c>
       <c r="B5"/>
       <c r="C5"/>
-      <c r="D5" s="69">
+      <c r="D5" s="60">
         <v>6.0221408570000002E+23</v>
       </c>
       <c r="E5"/>
@@ -8108,12 +8076,11 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" style="16" customWidth="1"/>
     <col min="3" max="1025" width="8.83203125" style="16" customWidth="1"/>
     <col min="1026" max="1027" width="9" style="16" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="16"/>
@@ -8223,8 +8190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8280,8 +8246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8295,26 +8260,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="66" t="s">
+      <c r="G2" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="H2" s="64"/>
-      <c r="I2" s="66" t="s">
+      <c r="H2" s="67"/>
+      <c r="I2" s="69" t="s">
         <v>148</v>
       </c>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="Q2" s="67" t="s">
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="Q2" s="70" t="s">
         <v>149</v>
       </c>
-      <c r="R2" s="64"/>
-      <c r="S2" s="67" t="s">
+      <c r="R2" s="67"/>
+      <c r="S2" s="70" t="s">
         <v>150</v>
       </c>
-      <c r="T2" s="64"/>
+      <c r="T2" s="67"/>
     </row>
     <row r="3" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -8403,7 +8368,6 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8460,7 +8424,6 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8476,10 +8439,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="H2" s="64"/>
+      <c r="H2" s="67"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -8575,7 +8538,6 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8658,7 +8620,6 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8719,7 +8680,6 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8795,7 +8755,6 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8866,7 +8825,6 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8936,8 +8894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -9022,9 +8979,6 @@
   <dimension ref="A1:AMR9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -9065,19 +9019,19 @@
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
       <c r="G2" s="32"/>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="61"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="64"/>
       <c r="L2" s="32"/>
-      <c r="M2" s="62" t="s">
+      <c r="M2" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -11287,10 +11241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -11316,14 +11267,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -11406,7 +11357,6 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11500,9 +11450,6 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>